<commit_message>
Updated annotation check protocol to improve the way it's written.
</commit_message>
<xml_diff>
--- a/megalocytivirus_sequence_data.xlsx
+++ b/megalocytivirus_sequence_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="8_{BBE3224F-4570-4915-A6DB-5FBC4F9097C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A1C7D15-7219-4A73-845B-A6495B79B26D}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="8_{BBE3224F-4570-4915-A6DB-5FBC4F9097C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72327071-6A2F-43E4-AB4F-528E208F73B8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{CD6C468C-256F-45C2-B81B-3E7578C677C5}"/>
   </bookViews>
@@ -41712,9 +41712,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DAEBFD-78AC-4E24-A1EF-CD140122AED7}">
   <dimension ref="A1:Y545"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H189" sqref="H189"/>
+    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A182" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74178,51 +74178,51 @@
     <hyperlink ref="O482" r:id="rId6" tooltip="Persistent link using digital object identifier" xr:uid="{9FF34F63-0E5C-4000-B5AC-F3151A5770E6}"/>
     <hyperlink ref="O91" r:id="rId7" xr:uid="{B10D636D-180A-4A07-9727-2D44C3A35EA4}"/>
     <hyperlink ref="O10" r:id="rId8" xr:uid="{4DFCC98B-6675-47C2-9D64-6D2D8E87F24F}"/>
-    <hyperlink ref="O185" r:id="rId9" display="10.3354/dao03500" xr:uid="{970A3DBD-2CA0-47FF-9146-7327C707266E}"/>
-    <hyperlink ref="O13" r:id="rId10" xr:uid="{0C654127-2FC0-4680-9308-B0C7C6BF3232}"/>
-    <hyperlink ref="O26" r:id="rId11" xr:uid="{6E9A3021-FEBB-4C61-AAF6-5EE2A2139933}"/>
-    <hyperlink ref="O14" r:id="rId12" xr:uid="{247EF52C-EEDC-45E7-8754-D67C06C32B99}"/>
-    <hyperlink ref="O15" r:id="rId13" xr:uid="{220F617A-B59E-4A81-91E8-5A4BEF453BD3}"/>
-    <hyperlink ref="O16" r:id="rId14" xr:uid="{E31F582D-D7D2-467B-9212-9BB0DC8587B3}"/>
-    <hyperlink ref="O17" r:id="rId15" xr:uid="{29FC70D7-1C68-4B78-9301-C86D014D41FE}"/>
-    <hyperlink ref="O18" r:id="rId16" xr:uid="{56BE1597-0B70-417C-B931-B6717DA29768}"/>
-    <hyperlink ref="O19" r:id="rId17" xr:uid="{EDCA27AA-4A2C-4FA7-87AC-E571ED8B1546}"/>
-    <hyperlink ref="O20" r:id="rId18" xr:uid="{B6A4A144-C222-4B60-BB74-498CC7114C8C}"/>
-    <hyperlink ref="O21" r:id="rId19" xr:uid="{DE5EF46A-BEDE-4D78-B342-16EB4CDA094D}"/>
-    <hyperlink ref="O22" r:id="rId20" xr:uid="{B38EDD32-94D7-4319-A063-B1121802AEFD}"/>
-    <hyperlink ref="O23" r:id="rId21" xr:uid="{671A9A05-A8B3-4CE8-A1F1-45D7A7A59CB7}"/>
-    <hyperlink ref="O24" r:id="rId22" xr:uid="{E82A118C-1A94-41C3-B0C3-51683EAC45E3}"/>
-    <hyperlink ref="O25" r:id="rId23" xr:uid="{CEB90C8D-FFA3-4D9F-B0D7-37DAAAAA0625}"/>
-    <hyperlink ref="O27" r:id="rId24" xr:uid="{F4807A92-AC2F-4CF9-97EC-76E1F7BB5144}"/>
-    <hyperlink ref="O28" r:id="rId25" xr:uid="{4BF5591F-364A-4652-BE55-A83F068E5FF0}"/>
-    <hyperlink ref="O29" r:id="rId26" xr:uid="{BBCE336A-8744-4123-9D7B-BDC7A4E23FE3}"/>
-    <hyperlink ref="O30" r:id="rId27" xr:uid="{6AA65A27-A249-4143-BE6F-DC724F6EF0CA}"/>
-    <hyperlink ref="O31" r:id="rId28" xr:uid="{241CC239-6C7C-4001-96FF-EA907FA2C1A3}"/>
-    <hyperlink ref="O293" r:id="rId29" xr:uid="{F542AB75-865F-4044-89A5-5B4A960D0F3B}"/>
-    <hyperlink ref="O297" r:id="rId30" xr:uid="{7DC2A623-021E-4438-8D49-0AB77EFB641B}"/>
-    <hyperlink ref="O351" r:id="rId31" xr:uid="{367F57BD-268C-4C50-8AD0-A6803441B162}"/>
-    <hyperlink ref="O352" r:id="rId32" xr:uid="{18C89575-94BD-47E8-B65E-EF36DE2414F2}"/>
-    <hyperlink ref="O479" r:id="rId33" xr:uid="{1164A360-48D2-418D-BAF4-DA98BB866927}"/>
-    <hyperlink ref="O311" r:id="rId34" xr:uid="{4DD5F13B-8CAD-445B-8176-29285F8242F4}"/>
-    <hyperlink ref="O310" r:id="rId35" xr:uid="{80643CC8-4F21-4FEF-850B-6DA4B7557466}"/>
-    <hyperlink ref="O188" r:id="rId36" xr:uid="{E5F9D793-F9E7-46A6-9B31-2CC2DFB7DD29}"/>
-    <hyperlink ref="O49" r:id="rId37" xr:uid="{F123D9E3-B89D-4081-9B5C-D652B4182A8C}"/>
-    <hyperlink ref="O48" r:id="rId38" xr:uid="{F56AC6C1-2C94-4E0A-A50A-5968D80354F8}"/>
-    <hyperlink ref="O47" r:id="rId39" xr:uid="{EF4D35BE-F56B-4D08-BA74-2A28EB388D2E}"/>
-    <hyperlink ref="O46" r:id="rId40" xr:uid="{90C02ACB-AEA8-4F64-92B6-FF82CF9E563A}"/>
-    <hyperlink ref="O45" r:id="rId41" xr:uid="{2E67A22B-9565-4644-8A48-7953A03598FD}"/>
-    <hyperlink ref="O43" r:id="rId42" xr:uid="{7EC30C09-4140-43B3-8416-7E4B0F784F02}"/>
-    <hyperlink ref="O42" r:id="rId43" xr:uid="{FC04C1A2-761F-41F1-A699-DC1FE2748E52}"/>
-    <hyperlink ref="O41" r:id="rId44" xr:uid="{5C67D4CA-CD0F-4DD6-A4C5-3DC8DF7B3831}"/>
-    <hyperlink ref="O44" r:id="rId45" display="https://doi.org/10.1007/s00705-011-1017-9" xr:uid="{7AE5ACFC-378E-465F-AD6C-476CFA2000AC}"/>
-    <hyperlink ref="O40" r:id="rId46" xr:uid="{14CD9B5A-E800-4600-BEEB-1355C2A0AC34}"/>
-    <hyperlink ref="O39" r:id="rId47" xr:uid="{71D5F34B-B8CA-4EBB-BD85-70BD70073747}"/>
-    <hyperlink ref="O474" r:id="rId48" display="https://doi.org/10.1006/viro.1997.8456" xr:uid="{D468A506-05EE-4943-92E5-5D9BF6661C6E}"/>
-    <hyperlink ref="O90" r:id="rId49" tooltip="PubMed" display="https://www.ncbi.nlm.nih.gov/pubmed?term=28928367+OR+29181623" xr:uid="{31CC3834-3FE5-4646-A9A7-5E79034796EF}"/>
-    <hyperlink ref="O92" r:id="rId50" tooltip="PubMed" display="https://www.ncbi.nlm.nih.gov/pubmed?term=16789247+OR+3959991+OR+2820141+OR+3201750+OR+1549908+OR+1475907+OR+8492091+OR+7698884+OR+8121799+OR+8073636+OR+8021587+OR+9482589+OR+9926400+OR+10456793+OR+11448171" xr:uid="{B5DB3097-7B00-2A4A-8AB3-111209C0C369}"/>
-    <hyperlink ref="O12" r:id="rId51" xr:uid="{127A5116-EDC0-49BD-BE3B-40FADE1D1524}"/>
-    <hyperlink ref="R92" r:id="rId52" tooltip="PubMed" display="https://www.ncbi.nlm.nih.gov/pubmed?term=16789247+OR+3959991+OR+2820141+OR+3201750+OR+1549908+OR+1475907+OR+8492091+OR+7698884+OR+8121799+OR+8073636+OR+8021587+OR+9482589+OR+9926400+OR+10456793+OR+11448171" xr:uid="{3FEC8D3C-95EF-49C8-9008-07A50A777F6F}"/>
-    <hyperlink ref="O485" r:id="rId53" location=":~:text=Whole-genome%20sequences%20of%20RISV-I%20type%20SBIV-VP13%20and%20RSIV-II" xr:uid="{CD7760A6-BED3-466B-80B4-5C0FB826986C}"/>
+    <hyperlink ref="O13" r:id="rId9" xr:uid="{0C654127-2FC0-4680-9308-B0C7C6BF3232}"/>
+    <hyperlink ref="O26" r:id="rId10" xr:uid="{6E9A3021-FEBB-4C61-AAF6-5EE2A2139933}"/>
+    <hyperlink ref="O14" r:id="rId11" xr:uid="{247EF52C-EEDC-45E7-8754-D67C06C32B99}"/>
+    <hyperlink ref="O15" r:id="rId12" xr:uid="{220F617A-B59E-4A81-91E8-5A4BEF453BD3}"/>
+    <hyperlink ref="O16" r:id="rId13" xr:uid="{E31F582D-D7D2-467B-9212-9BB0DC8587B3}"/>
+    <hyperlink ref="O17" r:id="rId14" xr:uid="{29FC70D7-1C68-4B78-9301-C86D014D41FE}"/>
+    <hyperlink ref="O18" r:id="rId15" xr:uid="{56BE1597-0B70-417C-B931-B6717DA29768}"/>
+    <hyperlink ref="O19" r:id="rId16" xr:uid="{EDCA27AA-4A2C-4FA7-87AC-E571ED8B1546}"/>
+    <hyperlink ref="O20" r:id="rId17" xr:uid="{B6A4A144-C222-4B60-BB74-498CC7114C8C}"/>
+    <hyperlink ref="O21" r:id="rId18" xr:uid="{DE5EF46A-BEDE-4D78-B342-16EB4CDA094D}"/>
+    <hyperlink ref="O22" r:id="rId19" xr:uid="{B38EDD32-94D7-4319-A063-B1121802AEFD}"/>
+    <hyperlink ref="O23" r:id="rId20" xr:uid="{671A9A05-A8B3-4CE8-A1F1-45D7A7A59CB7}"/>
+    <hyperlink ref="O24" r:id="rId21" xr:uid="{E82A118C-1A94-41C3-B0C3-51683EAC45E3}"/>
+    <hyperlink ref="O25" r:id="rId22" xr:uid="{CEB90C8D-FFA3-4D9F-B0D7-37DAAAAA0625}"/>
+    <hyperlink ref="O27" r:id="rId23" xr:uid="{F4807A92-AC2F-4CF9-97EC-76E1F7BB5144}"/>
+    <hyperlink ref="O28" r:id="rId24" xr:uid="{4BF5591F-364A-4652-BE55-A83F068E5FF0}"/>
+    <hyperlink ref="O29" r:id="rId25" xr:uid="{BBCE336A-8744-4123-9D7B-BDC7A4E23FE3}"/>
+    <hyperlink ref="O30" r:id="rId26" xr:uid="{6AA65A27-A249-4143-BE6F-DC724F6EF0CA}"/>
+    <hyperlink ref="O31" r:id="rId27" xr:uid="{241CC239-6C7C-4001-96FF-EA907FA2C1A3}"/>
+    <hyperlink ref="O293" r:id="rId28" xr:uid="{F542AB75-865F-4044-89A5-5B4A960D0F3B}"/>
+    <hyperlink ref="O297" r:id="rId29" xr:uid="{7DC2A623-021E-4438-8D49-0AB77EFB641B}"/>
+    <hyperlink ref="O351" r:id="rId30" xr:uid="{367F57BD-268C-4C50-8AD0-A6803441B162}"/>
+    <hyperlink ref="O352" r:id="rId31" xr:uid="{18C89575-94BD-47E8-B65E-EF36DE2414F2}"/>
+    <hyperlink ref="O479" r:id="rId32" xr:uid="{1164A360-48D2-418D-BAF4-DA98BB866927}"/>
+    <hyperlink ref="O311" r:id="rId33" xr:uid="{4DD5F13B-8CAD-445B-8176-29285F8242F4}"/>
+    <hyperlink ref="O310" r:id="rId34" xr:uid="{80643CC8-4F21-4FEF-850B-6DA4B7557466}"/>
+    <hyperlink ref="O188" r:id="rId35" xr:uid="{E5F9D793-F9E7-46A6-9B31-2CC2DFB7DD29}"/>
+    <hyperlink ref="O49" r:id="rId36" xr:uid="{F123D9E3-B89D-4081-9B5C-D652B4182A8C}"/>
+    <hyperlink ref="O48" r:id="rId37" xr:uid="{F56AC6C1-2C94-4E0A-A50A-5968D80354F8}"/>
+    <hyperlink ref="O47" r:id="rId38" xr:uid="{EF4D35BE-F56B-4D08-BA74-2A28EB388D2E}"/>
+    <hyperlink ref="O46" r:id="rId39" xr:uid="{90C02ACB-AEA8-4F64-92B6-FF82CF9E563A}"/>
+    <hyperlink ref="O45" r:id="rId40" xr:uid="{2E67A22B-9565-4644-8A48-7953A03598FD}"/>
+    <hyperlink ref="O43" r:id="rId41" xr:uid="{7EC30C09-4140-43B3-8416-7E4B0F784F02}"/>
+    <hyperlink ref="O42" r:id="rId42" xr:uid="{FC04C1A2-761F-41F1-A699-DC1FE2748E52}"/>
+    <hyperlink ref="O41" r:id="rId43" xr:uid="{5C67D4CA-CD0F-4DD6-A4C5-3DC8DF7B3831}"/>
+    <hyperlink ref="O44" r:id="rId44" display="https://doi.org/10.1007/s00705-011-1017-9" xr:uid="{7AE5ACFC-378E-465F-AD6C-476CFA2000AC}"/>
+    <hyperlink ref="O40" r:id="rId45" xr:uid="{14CD9B5A-E800-4600-BEEB-1355C2A0AC34}"/>
+    <hyperlink ref="O39" r:id="rId46" xr:uid="{71D5F34B-B8CA-4EBB-BD85-70BD70073747}"/>
+    <hyperlink ref="O474" r:id="rId47" display="https://doi.org/10.1006/viro.1997.8456" xr:uid="{D468A506-05EE-4943-92E5-5D9BF6661C6E}"/>
+    <hyperlink ref="O90" r:id="rId48" tooltip="PubMed" display="https://www.ncbi.nlm.nih.gov/pubmed?term=28928367+OR+29181623" xr:uid="{31CC3834-3FE5-4646-A9A7-5E79034796EF}"/>
+    <hyperlink ref="O92" r:id="rId49" tooltip="PubMed" display="https://www.ncbi.nlm.nih.gov/pubmed?term=16789247+OR+3959991+OR+2820141+OR+3201750+OR+1549908+OR+1475907+OR+8492091+OR+7698884+OR+8121799+OR+8073636+OR+8021587+OR+9482589+OR+9926400+OR+10456793+OR+11448171" xr:uid="{B5DB3097-7B00-2A4A-8AB3-111209C0C369}"/>
+    <hyperlink ref="O12" r:id="rId50" xr:uid="{127A5116-EDC0-49BD-BE3B-40FADE1D1524}"/>
+    <hyperlink ref="R92" r:id="rId51" tooltip="PubMed" display="https://www.ncbi.nlm.nih.gov/pubmed?term=16789247+OR+3959991+OR+2820141+OR+3201750+OR+1549908+OR+1475907+OR+8492091+OR+7698884+OR+8121799+OR+8073636+OR+8021587+OR+9482589+OR+9926400+OR+10456793+OR+11448171" xr:uid="{3FEC8D3C-95EF-49C8-9008-07A50A777F6F}"/>
+    <hyperlink ref="O485" r:id="rId52" location=":~:text=Whole-genome%20sequences%20of%20RISV-I%20type%20SBIV-VP13%20and%20RSIV-II" xr:uid="{CD7760A6-BED3-466B-80B4-5C0FB826986C}"/>
+    <hyperlink ref="O185" r:id="rId53" display="10.3354/dao03500" xr:uid="{970A3DBD-2CA0-47FF-9146-7327C707266E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>

</xml_diff>

<commit_message>
Updated spreadsheet with additional Megalocytivirus genomes now added.
</commit_message>
<xml_diff>
--- a/megalocytivirus_sequence_data.xlsx
+++ b/megalocytivirus_sequence_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="8_{BBE3224F-4570-4915-A6DB-5FBC4F9097C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72327071-6A2F-43E4-AB4F-528E208F73B8}"/>
+  <xr:revisionPtr revIDLastSave="726" documentId="8_{BBE3224F-4570-4915-A6DB-5FBC4F9097C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62B88E9B-FBA9-4D98-B230-C75292189FBB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{CD6C468C-256F-45C2-B81B-3E7578C677C5}"/>
   </bookViews>
@@ -47,8 +47,10 @@
     <author>tc={8565A256-F193-4C83-A615-E4C46246823E}</author>
     <author>tc={8628BEEB-50F7-4F49-9929-1B9449FC2F0D}</author>
     <author>tc={9722C737-1158-4501-8B63-465162F6E8DF}</author>
+    <author>tc={406640DC-9DBB-462C-958D-EDF23513ABFA}</author>
     <author>tc={5230F35F-320F-4232-83AC-E9E62C3EAF99}</author>
     <author>tc={E215A2BB-47F3-4A44-A7C6-FD44B413BC51}</author>
+    <author>tc={E1CCBB3F-E5CC-4052-BACF-543F5E11D8D4}</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{01BE6336-2FEF-48C6-9E5A-9F4513FC308D}">
@@ -116,7 +118,15 @@
     This study published the RSIV genotype too. Although, this publication is not mentioned on NCBI.</t>
       </text>
     </comment>
-    <comment ref="H264" authorId="6" shapeId="0" xr:uid="{5230F35F-320F-4232-83AC-E9E62C3EAF99}">
+    <comment ref="H189" authorId="6" shapeId="0" xr:uid="{406640DC-9DBB-462C-958D-EDF23513ABFA}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Says partial in data field for GenBank entry but title and sequence length indicate the sequence is complete. </t>
+      </text>
+    </comment>
+    <comment ref="H264" authorId="7" shapeId="0" xr:uid="{5230F35F-320F-4232-83AC-E9E62C3EAF99}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -124,7 +134,7 @@
     Listed in Genbankas a partial sequence, but desribed in sequence inforomation as a 'Circular physical map of RSIV, Complete sequence'. The paper is in Japanese but by the look of the phylogeny there are not new sequences/genomes described in this paper. </t>
       </text>
     </comment>
-    <comment ref="V473" authorId="7" shapeId="0" xr:uid="{E215A2BB-47F3-4A44-A7C6-FD44B413BC51}">
+    <comment ref="V473" authorId="8" shapeId="0" xr:uid="{E215A2BB-47F3-4A44-A7C6-FD44B413BC51}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -132,12 +142,20 @@
     FYI: A BioProject is bunch of biological data related to a single initiative, originating from a single ogroup (organisation). It provides people with a central place to find links to the data types generated for that project. </t>
       </text>
     </comment>
+    <comment ref="M490" authorId="9" shapeId="0" xr:uid="{E1CCBB3F-E5CC-4052-BACF-543F5E11D8D4}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Laboratory host. </t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9370" uniqueCount="1881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9822" uniqueCount="1970">
   <si>
     <t>Species</t>
   </si>
@@ -40211,47 +40229,6 @@
   </si>
   <si>
     <r>
-      <t>Yes - '</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A Maximal likelihood phylogenetic analysis was carried out
-using the concatenated sequences of 25 core proteins of IVs. Each protein was aligned separately using Muscle Web Server  The alignments were trimmed using TrimAl 1.3 to remove less conserved positions. The trimmed alignments of the 25 con_x0002_served proteins were then concatenated using Mesquite. An unrooted maximal likelihood tree was generated using PhyML 3.0 combined with Smart Model Selection. The LG+G+I+F model was identified as the optimal for maximal likeli_x0002_hood analysis in this case. A bootstrap test was carried out
-with 500 replicates.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">I think this may be in fact be a decapodirivovirus. The decapodiridovirus has not yet been establishedwhen this paper was writte. There is a whole genome available for decapodiridovirus with accession number: MF59946. Perhaps this one just has not been classified in GenBank yet as decapodiridovirus.  </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -41040,13 +41017,320 @@
   </si>
   <si>
     <t>lymphocystis disease virus 1</t>
+  </si>
+  <si>
+    <t>MW883598</t>
+  </si>
+  <si>
+    <t>RSIV-HGIV-Cantik-2014</t>
+  </si>
+  <si>
+    <t>The University of Sydney, School of Life and Environmental Sciences</t>
+  </si>
+  <si>
+    <t>Epinephelus fuscoguttatus x Epinephelus polyphekadion</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1155/2023/6643006</t>
+  </si>
+  <si>
+    <t>PP151097</t>
+  </si>
+  <si>
+    <t>ISKNV-ASB-23</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.20944/preprints202407.1210.v1</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>The Co-infection of ISKNV-II and RGNNV Resulting in Mass Mortalities of Juvenile Asian Seabass (Lates calcarifer), Zhuhai, Southern China - [v1]</t>
+  </si>
+  <si>
+    <t>ON212400</t>
+  </si>
+  <si>
+    <t>TIV-2020</t>
+  </si>
+  <si>
+    <t>University of Florida, Department of Infectious Diseases and Pathology</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Tilapia</t>
+  </si>
+  <si>
+    <t>OR670976</t>
+  </si>
+  <si>
+    <t>ISKNV_Ghana_TIV_2019</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>MW883595</t>
+  </si>
+  <si>
+    <t>BCIV-2015</t>
+  </si>
+  <si>
+    <t>MT128667</t>
+  </si>
+  <si>
+    <t>KU2</t>
+  </si>
+  <si>
+    <t>Kasetsart University, Department of Aquaculture</t>
+  </si>
+  <si>
+    <t>MW883606</t>
+  </si>
+  <si>
+    <t>OGIV-PW-2018</t>
+  </si>
+  <si>
+    <t>MT128666</t>
+  </si>
+  <si>
+    <t>KU1</t>
+  </si>
+  <si>
+    <t>MW273354</t>
+  </si>
+  <si>
+    <t>EFIV-2019</t>
+  </si>
+  <si>
+    <t>University of Florida, Infectious Diseases and Immunology</t>
+  </si>
+  <si>
+    <t>MW273353</t>
+  </si>
+  <si>
+    <t> EFIV-2018</t>
+  </si>
+  <si>
+    <t>NC_003494</t>
+  </si>
+  <si>
+    <t>National Center for Biotechnology Information, NIH</t>
+  </si>
+  <si>
+    <t>Mandarin fish (Siniperca chuatsi)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1006%2Fviro.2001.1208</t>
+  </si>
+  <si>
+    <t>OQ513807</t>
+  </si>
+  <si>
+    <t>LakeVolta_BF-2</t>
+  </si>
+  <si>
+    <t>University of Exeter, Biosciences</t>
+  </si>
+  <si>
+    <t>10.3390/v15040965</t>
+  </si>
+  <si>
+    <t>MW883599</t>
+  </si>
+  <si>
+    <t>TTIV-2015</t>
+  </si>
+  <si>
+    <t>Tilapia (Oreochromis niloticus)</t>
+  </si>
+  <si>
+    <t>The three spot gourami (Trichopodus trichopterus)</t>
+  </si>
+  <si>
+    <t>Rainbow shark (Epalzeorhynchos frenatum)</t>
+  </si>
+  <si>
+    <t>Giant gourami (Osphronemus goramy)</t>
+  </si>
+  <si>
+    <t>Barramundi (Lates calcarifer)</t>
+  </si>
+  <si>
+    <t>Banggai cardinalfish (Pterapogon kauderni)</t>
+  </si>
+  <si>
+    <t>OP896201</t>
+  </si>
+  <si>
+    <t>NH-2005</t>
+  </si>
+  <si>
+    <t>Sun Yat-Sen University, School of Marine Science</t>
+  </si>
+  <si>
+    <t>OR356116</t>
+  </si>
+  <si>
+    <t>MW883593</t>
+  </si>
+  <si>
+    <t>TLIV-2011</t>
+  </si>
+  <si>
+    <t>NH-2021</t>
+  </si>
+  <si>
+    <t>KT781098</t>
+  </si>
+  <si>
+    <t>Red seabream (Pagrus major)</t>
+  </si>
+  <si>
+    <t>MW883603</t>
+  </si>
+  <si>
+    <t>HGIV-2015</t>
+  </si>
+  <si>
+    <t>MW883596</t>
+  </si>
+  <si>
+    <t>HGIV-Cantik1-2014</t>
+  </si>
+  <si>
+    <t>MW883597</t>
+  </si>
+  <si>
+    <t>HGIV-Cantik2-2014</t>
+  </si>
+  <si>
+    <t>MW883601</t>
+  </si>
+  <si>
+    <t>TLIV-2015</t>
+  </si>
+  <si>
+    <t>Dwarf gourmani (Trichogaster lalius)</t>
+  </si>
+  <si>
+    <t>MW883602</t>
+  </si>
+  <si>
+    <t>XMIV-2015</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Southern platysfish (Xiphophorus maculatus)</t>
+  </si>
+  <si>
+    <t>MW883600</t>
+  </si>
+  <si>
+    <t>XHIV-2015</t>
+  </si>
+  <si>
+    <t> 110894</t>
+  </si>
+  <si>
+    <t>Green swordtail (Xiphophorus hellerii)</t>
+  </si>
+  <si>
+    <t>PP974677</t>
+  </si>
+  <si>
+    <t>OGIV-HN-2018-001</t>
+  </si>
+  <si>
+    <t>College of Marine Sciences, South China Agricultural University</t>
+  </si>
+  <si>
+    <t>Giant groper (Epinephelus lanceolatus)</t>
+  </si>
+  <si>
+    <t>OR536350</t>
+  </si>
+  <si>
+    <t>AK-ISKNV</t>
+  </si>
+  <si>
+    <t>College of Fisheries, KVAFSU Bidar, Department of Aquatic Animal Health Management</t>
+  </si>
+  <si>
+    <t>Angelfish (Pterophyllum scalare)</t>
+  </si>
+  <si>
+    <t>MW883594</t>
+  </si>
+  <si>
+    <t>TTIV-2011</t>
+  </si>
+  <si>
+    <t>Blue gourami (Trichopodus trichopterus)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">I think this may be in fact be a decapodirivovirus. The decapodiridovirus has not yet been establishedwhen this paper was writte. There is a whole genome available for decapodiridovirus with accession number: MF59946. Perhaps this one just has not been classified in GenBank yet as decapodiridovirus.  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Yes - '</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Maximal likelihood phylogenetic analysis was carried out
+using the concatenated sequences of 25 core proteins of IVs. Each protein was aligned separately using Muscle Web Server  The alignments were trimmed using TrimAl 1.3 to remove less conserved positions. The trimmed alignments of the 25 con_x0002_served proteins were then concatenated using Mesquite. An unrooted maximal likelihood tree was generated using PhyML 3.0 combined with Smart Model Selection. The LG+G+I+F model was identified as the optimal for maximal likeli_x0002_hood analysis in this case. A bootstrap test was carried out
+with 500 replicates.</t>
+    </r>
+  </si>
+  <si>
+    <t>Not yet published (pre-print)</t>
+  </si>
+  <si>
+    <t>Fusianto</t>
+  </si>
+  <si>
+    <t>Genotypic Characterization of Infectious Spleen and Kidney Necrosis Virus (ISKNV) in Southeast Asian Aquaculture</t>
+  </si>
+  <si>
+    <t>I have not yet completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41196,6 +41480,26 @@
       <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -41230,7 +41534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -41339,6 +41643,40 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -41699,11 +42037,17 @@
   <threadedComment ref="Q185" dT="2024-08-05T02:25:11.87" personId="{87A94ADC-9B33-4CC6-9B4A-A7607D916083}" id="{9722C737-1158-4501-8B63-465162F6E8DF}">
     <text>This study published the RSIV genotype too. Although, this publication is not mentioned on NCBI.</text>
   </threadedComment>
+  <threadedComment ref="H189" dT="2025-01-02T04:07:05.68" personId="{87A94ADC-9B33-4CC6-9B4A-A7607D916083}" id="{406640DC-9DBB-462C-958D-EDF23513ABFA}">
+    <text xml:space="preserve">Says partial in data field for GenBank entry but title and sequence length indicate the sequence is complete. </text>
+  </threadedComment>
   <threadedComment ref="H264" dT="2024-03-13T00:39:43.73" personId="{D62592C3-9826-4F3A-8754-81789E0904D2}" id="{5230F35F-320F-4232-83AC-E9E62C3EAF99}">
     <text xml:space="preserve">Listed in Genbankas a partial sequence, but desribed in sequence inforomation as a 'Circular physical map of RSIV, Complete sequence'. The paper is in Japanese but by the look of the phylogeny there are not new sequences/genomes described in this paper. </text>
   </threadedComment>
   <threadedComment ref="V473" dT="2024-03-25T00:59:42.03" personId="{D62592C3-9826-4F3A-8754-81789E0904D2}" id="{E215A2BB-47F3-4A44-A7C6-FD44B413BC51}">
     <text xml:space="preserve">FYI: A BioProject is bunch of biological data related to a single initiative, originating from a single ogroup (organisation). It provides people with a central place to find links to the data types generated for that project. </text>
+  </threadedComment>
+  <threadedComment ref="M490" dT="2025-01-02T04:10:55.75" personId="{87A94ADC-9B33-4CC6-9B4A-A7607D916083}" id="{E1CCBB3F-E5CC-4052-BACF-543F5E11D8D4}">
+    <text xml:space="preserve">Laboratory host. </text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -41712,9 +42056,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DAEBFD-78AC-4E24-A1EF-CD140122AED7}">
   <dimension ref="A1:Y545"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A182" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A498" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A512" sqref="A512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41829,7 +42173,7 @@
         <v>1663</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>1865</v>
+        <v>1863</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>1622</v>
@@ -41951,7 +42295,7 @@
         <v>1387</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>1826</v>
+        <v>1824</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>26</v>
@@ -42022,7 +42366,7 @@
         <v>1395</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>1827</v>
+        <v>1825</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>25</v>
@@ -42048,7 +42392,7 @@
         <v>1663</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>1866</v>
+        <v>1864</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>1616</v>
@@ -42170,7 +42514,7 @@
         <v>1393</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>1828</v>
+        <v>1826</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>29</v>
@@ -42309,7 +42653,7 @@
         <v>7</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="R8" s="3">
         <v>2002</v>
@@ -42318,7 +42662,7 @@
         <v>1385</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>1386</v>
@@ -42601,7 +42945,7 @@
         <v>1701</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>1830</v>
+        <v>1828</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>841</v>
@@ -47648,7 +47992,7 @@
         <v>1664</v>
       </c>
       <c r="D90" s="34" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
       <c r="E90" s="20" t="s">
         <v>1609</v>
@@ -47687,7 +48031,7 @@
         <v>1811</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="R90" s="2" t="s">
         <v>1776</v>
@@ -47796,7 +48140,7 @@
         <v>1662</v>
       </c>
       <c r="D92" s="34" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="E92" s="20" t="s">
         <v>1651</v>
@@ -48000,7 +48344,7 @@
         <v>1662</v>
       </c>
       <c r="D95" s="34" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="E95" s="20" t="s">
         <v>1614</v>
@@ -48206,10 +48550,10 @@
         <v>1750</v>
       </c>
       <c r="D98" s="34" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="F98" s="8" t="s">
         <v>1581</v>
@@ -48230,7 +48574,7 @@
         <v>1569</v>
       </c>
       <c r="N98" s="10" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="O98" s="2" t="s">
         <v>1572</v>
@@ -50709,13 +51053,13 @@
         <v>2016</v>
       </c>
       <c r="O135" s="2" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="P135" s="6" t="s">
+        <v>1839</v>
+      </c>
+      <c r="Q135" s="2" t="s">
         <v>1841</v>
-      </c>
-      <c r="Q135" s="2" t="s">
-        <v>1843</v>
       </c>
       <c r="R135" s="11" t="s">
         <v>7</v>
@@ -50753,7 +51097,7 @@
         <v>1678</v>
       </c>
       <c r="E136" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
       <c r="F136" t="s">
         <v>1560</v>
@@ -50783,13 +51127,13 @@
         <v>2016</v>
       </c>
       <c r="O136" s="4" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="P136" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="Q136" s="2" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="R136" s="3">
         <v>2020</v>
@@ -59406,7 +59750,7 @@
       </c>
       <c r="S268" s="10"/>
       <c r="T268" s="2" t="s">
-        <v>1836</v>
+        <v>1834</v>
       </c>
       <c r="U268" s="2" t="s">
         <v>767</v>
@@ -59538,7 +59882,7 @@
       </c>
       <c r="S270" s="10"/>
       <c r="T270" s="2" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="U270" s="2" t="s">
         <v>774</v>
@@ -61338,7 +61682,7 @@
         <v>2011</v>
       </c>
       <c r="T297" s="2" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
       <c r="U297" s="2" t="s">
         <v>174</v>
@@ -62982,7 +63326,7 @@
         <v>2014</v>
       </c>
       <c r="T322" s="9" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="U322" s="2" t="s">
         <v>918</v>
@@ -63384,7 +63728,7 @@
         <v>933</v>
       </c>
       <c r="V328" s="2" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="329" spans="1:24" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -63449,7 +63793,7 @@
         <v>933</v>
       </c>
       <c r="V329" s="2" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="330" spans="1:24" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -63514,7 +63858,7 @@
         <v>933</v>
       </c>
       <c r="V330" s="2" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="331" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
@@ -65470,13 +65814,13 @@
         <v>43118</v>
       </c>
       <c r="O360" s="2" t="s">
+        <v>1858</v>
+      </c>
+      <c r="P360" s="6" t="s">
+        <v>1859</v>
+      </c>
+      <c r="Q360" s="2" t="s">
         <v>1860</v>
-      </c>
-      <c r="P360" s="6" t="s">
-        <v>1861</v>
-      </c>
-      <c r="Q360" s="2" t="s">
-        <v>1862</v>
       </c>
       <c r="R360" s="11" t="s">
         <v>7</v>
@@ -65612,25 +65956,25 @@
         <v>1515</v>
       </c>
       <c r="O362" s="2" t="s">
+        <v>1842</v>
+      </c>
+      <c r="P362" s="6" t="s">
+        <v>1843</v>
+      </c>
+      <c r="Q362" s="2" t="s">
         <v>1844</v>
-      </c>
-      <c r="P362" s="6" t="s">
-        <v>1845</v>
-      </c>
-      <c r="Q362" s="2" t="s">
-        <v>1846</v>
       </c>
       <c r="R362" s="11">
         <v>2022</v>
       </c>
       <c r="S362" s="2" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="T362" s="2" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="U362" s="2" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="V362" s="2" t="s">
         <v>315</v>
@@ -66435,7 +66779,7 @@
         <v>1750</v>
       </c>
       <c r="D375" s="34" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="E375" s="36" t="s">
         <v>1592</v>
@@ -66684,7 +67028,7 @@
         <v>1702</v>
       </c>
       <c r="T378" s="2" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="U378" s="2" t="s">
         <v>1072</v>
@@ -70504,25 +70848,25 @@
         <v>1186</v>
       </c>
       <c r="M437" s="8" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="N437" s="8">
         <v>2017</v>
       </c>
       <c r="O437" s="2" t="s">
+        <v>1846</v>
+      </c>
+      <c r="P437" s="6" t="s">
+        <v>1847</v>
+      </c>
+      <c r="Q437" s="2" t="s">
         <v>1848</v>
-      </c>
-      <c r="P437" s="6" t="s">
-        <v>1849</v>
-      </c>
-      <c r="Q437" s="2" t="s">
-        <v>1850</v>
       </c>
       <c r="R437" s="11">
         <v>2021</v>
       </c>
       <c r="S437" s="11" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="T437" s="2" t="s">
         <v>7</v>
@@ -70575,31 +70919,31 @@
         <v>1448</v>
       </c>
       <c r="M438" s="8" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
       <c r="N438" s="29">
         <v>2017</v>
       </c>
       <c r="O438" s="2" t="s">
+        <v>1851</v>
+      </c>
+      <c r="P438" s="6" t="s">
+        <v>1847</v>
+      </c>
+      <c r="Q438" s="2" t="s">
+        <v>1850</v>
+      </c>
+      <c r="R438" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="S438" s="11" t="s">
+        <v>1852</v>
+      </c>
+      <c r="T438" s="2" t="s">
         <v>1853</v>
       </c>
-      <c r="P438" s="6" t="s">
-        <v>1849</v>
-      </c>
-      <c r="Q438" s="2" t="s">
-        <v>1852</v>
-      </c>
-      <c r="R438" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="S438" s="11" t="s">
+      <c r="U438" s="2" t="s">
         <v>1854</v>
-      </c>
-      <c r="T438" s="2" t="s">
-        <v>1855</v>
-      </c>
-      <c r="U438" s="2" t="s">
-        <v>1856</v>
       </c>
       <c r="V438" s="2" t="s">
         <v>616</v>
@@ -72472,7 +72816,7 @@
         <v>1349</v>
       </c>
       <c r="D467" s="34" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="E467" s="36" t="s">
         <v>1647</v>
@@ -72540,7 +72884,7 @@
         <v>1349</v>
       </c>
       <c r="D468" s="50" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="E468" s="36" t="s">
         <v>1649</v>
@@ -72602,7 +72946,7 @@
         <v>1349</v>
       </c>
       <c r="D469" s="51" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
       <c r="E469" s="38" t="s">
         <v>1630</v>
@@ -72670,7 +73014,7 @@
         <v>1349</v>
       </c>
       <c r="D470" s="36" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="E470" s="20" t="s">
         <v>1623</v>
@@ -72878,7 +73222,7 @@
         <v>1349</v>
       </c>
       <c r="D473" s="1" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="E473" t="s">
         <v>1357</v>
@@ -72947,7 +73291,7 @@
         <v>1750</v>
       </c>
       <c r="D474" s="34" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="E474" t="s">
         <v>1361</v>
@@ -73077,7 +73421,7 @@
         <v>1750</v>
       </c>
       <c r="D476" s="34" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="E476" t="s">
         <v>1583</v>
@@ -73148,7 +73492,7 @@
         <v>1349</v>
       </c>
       <c r="D477" s="36" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="E477" s="38" t="s">
         <v>1644</v>
@@ -73361,7 +73705,7 @@
         <v>1663</v>
       </c>
       <c r="D480" s="36" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="E480" s="20" t="s">
         <v>1635</v>
@@ -73430,7 +73774,7 @@
         <v>1663</v>
       </c>
       <c r="D481" s="36" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="E481" s="20" t="s">
         <v>1627</v>
@@ -73566,7 +73910,7 @@
         <v>1349</v>
       </c>
       <c r="D483" s="1" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="E483" t="s">
         <v>1350</v>
@@ -73620,7 +73964,7 @@
         <v>1355</v>
       </c>
       <c r="V483" s="2" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="W483" s="2" t="s">
         <v>1381</v>
@@ -73744,13 +74088,13 @@
         <v>2020</v>
       </c>
       <c r="O485" s="43" t="s">
-        <v>1859</v>
+        <v>1857</v>
       </c>
       <c r="P485" s="6" t="s">
         <v>1080</v>
       </c>
       <c r="Q485" s="2" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
       <c r="R485" s="11" t="s">
         <v>7</v>
@@ -73916,195 +74260,1887 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="488" spans="1:24" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A488" t="s">
+    <row r="488" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A488" s="57" t="s">
         <v>1813</v>
       </c>
-      <c r="B488" t="s">
+      <c r="B488" s="57" t="s">
         <v>1749</v>
       </c>
-      <c r="C488" t="s">
+      <c r="C488" s="57" t="s">
         <v>1814</v>
       </c>
-      <c r="D488" t="s">
+      <c r="D488" s="57" t="s">
         <v>1294</v>
       </c>
-      <c r="E488" t="s">
+      <c r="E488" s="57" t="s">
         <v>1815</v>
       </c>
-      <c r="G488" t="s">
+      <c r="F488" s="57"/>
+      <c r="G488" s="57" t="s">
         <v>1816</v>
       </c>
-      <c r="H488" s="8" t="s">
+      <c r="H488" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I488">
+      <c r="I488" s="57">
         <v>165695</v>
       </c>
-      <c r="J488" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K488" s="2" t="s">
+      <c r="J488" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K488" s="59" t="s">
         <v>1817</v>
       </c>
-      <c r="L488" s="2" t="s">
+      <c r="L488" s="59" t="s">
         <v>941</v>
       </c>
-      <c r="M488" s="2" t="s">
+      <c r="M488" s="59" t="s">
         <v>1818</v>
       </c>
-      <c r="N488" s="10" t="s">
+      <c r="N488" s="60" t="s">
         <v>1819</v>
       </c>
-      <c r="O488" s="2" t="s">
+      <c r="O488" s="59" t="s">
         <v>1820</v>
       </c>
-      <c r="P488" s="6" t="s">
+      <c r="P488" s="61" t="s">
         <v>1821</v>
       </c>
-      <c r="Q488" s="2" t="s">
+      <c r="Q488" s="59" t="s">
         <v>1822</v>
       </c>
-      <c r="R488" s="3">
+      <c r="R488" s="62">
         <v>2017</v>
       </c>
-      <c r="S488" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="T488" s="2" t="s">
-        <v>1823</v>
-      </c>
-      <c r="V488" s="2" t="s">
-        <v>1824</v>
-      </c>
+      <c r="S488" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T488" s="59" t="s">
+        <v>1965</v>
+      </c>
+      <c r="U488" s="59"/>
+      <c r="V488" s="54" t="s">
+        <v>1964</v>
+      </c>
+      <c r="W488" s="52"/>
     </row>
-    <row r="489" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H489" s="8"/>
+    <row r="489" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A489" s="57" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B489" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C489" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D489" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E489" s="57" t="s">
+        <v>1880</v>
+      </c>
+      <c r="F489" s="57" t="s">
+        <v>1361</v>
+      </c>
+      <c r="G489" s="57" t="s">
+        <v>1880</v>
+      </c>
+      <c r="H489" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I489" s="57">
+        <v>112717</v>
+      </c>
+      <c r="J489" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K489" s="59" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L489" s="59" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M489" s="59" t="s">
+        <v>1882</v>
+      </c>
+      <c r="N489" s="60">
+        <v>2014</v>
+      </c>
+      <c r="O489" s="64" t="s">
+        <v>1883</v>
+      </c>
+      <c r="P489" s="57"/>
+      <c r="Q489" s="59"/>
+      <c r="R489" s="62"/>
+      <c r="S489" s="62"/>
+      <c r="T489" s="59"/>
+      <c r="U489" s="59"/>
+      <c r="V489" s="52"/>
+      <c r="W489" s="52"/>
     </row>
-    <row r="490" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H490" s="8"/>
+    <row r="490" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A490" s="57" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B490" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C490" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D490" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E490" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F490" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G490" s="57" t="s">
+        <v>1885</v>
+      </c>
+      <c r="H490" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I490" s="57">
+        <v>112236</v>
+      </c>
+      <c r="J490" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K490" s="57" t="s">
+        <v>1447</v>
+      </c>
+      <c r="L490" s="59" t="s">
+        <v>941</v>
+      </c>
+      <c r="M490" s="59" t="s">
+        <v>952</v>
+      </c>
+      <c r="N490" s="60">
+        <v>2023</v>
+      </c>
+      <c r="O490" s="59" t="s">
+        <v>1886</v>
+      </c>
+      <c r="P490" s="59" t="s">
+        <v>1887</v>
+      </c>
+      <c r="Q490" s="59" t="s">
+        <v>1888</v>
+      </c>
+      <c r="R490" s="62" t="s">
+        <v>1966</v>
+      </c>
+      <c r="S490" s="62"/>
+      <c r="T490" s="59"/>
+      <c r="U490" s="59"/>
+      <c r="V490" s="52"/>
+      <c r="W490" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="491" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H491" s="8"/>
+      <c r="A491" s="57" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B491" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C491" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D491" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E491" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F491" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G491" s="57" t="s">
+        <v>1890</v>
+      </c>
+      <c r="H491" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I491" s="57">
+        <v>111837</v>
+      </c>
+      <c r="J491" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K491" s="57" t="s">
+        <v>1891</v>
+      </c>
+      <c r="L491" s="59" t="s">
+        <v>1892</v>
+      </c>
+      <c r="M491" s="59" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N491" s="60">
+        <v>2020</v>
+      </c>
+      <c r="O491" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P491" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q491" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="R491" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="S491" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="T491" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="U491" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="V491" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W491" s="54" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="492" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H492" s="8"/>
+      <c r="A492" s="57" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B492" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C492" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D492" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E492" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F492" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G492" s="57" t="s">
+        <v>1895</v>
+      </c>
+      <c r="H492" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I492" s="57">
+        <v>111831</v>
+      </c>
+      <c r="J492" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K492" s="57" t="s">
+        <v>1891</v>
+      </c>
+      <c r="L492" s="59" t="s">
+        <v>1896</v>
+      </c>
+      <c r="M492" s="59" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N492" s="60">
+        <v>2019</v>
+      </c>
+      <c r="O492" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P492" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q492" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="R492" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="S492" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="T492" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="U492" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="V492" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W492" s="54" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="493" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H493" s="8"/>
+    <row r="493" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A493" s="57" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B493" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C493" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D493" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E493" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F493" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G493" s="57" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H493" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I493" s="57">
+        <v>111666</v>
+      </c>
+      <c r="J493" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K493" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L493" s="59" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M493" s="57" t="s">
+        <v>1926</v>
+      </c>
+      <c r="N493" s="60">
+        <v>2015</v>
+      </c>
+      <c r="O493" s="65" t="s">
+        <v>1883</v>
+      </c>
+      <c r="P493" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q493" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R493" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S493" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T493" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U493" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V493" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W493" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="494" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H494" s="8"/>
+      <c r="A494" s="57" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B494" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C494" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D494" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E494" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F494" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G494" s="57" t="s">
+        <v>1900</v>
+      </c>
+      <c r="H494" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I494" s="57">
+        <v>111610</v>
+      </c>
+      <c r="J494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K494" s="57" t="s">
+        <v>1901</v>
+      </c>
+      <c r="L494" s="59" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M494" s="59" t="s">
+        <v>1925</v>
+      </c>
+      <c r="N494" s="60">
+        <v>2018</v>
+      </c>
+      <c r="O494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="R494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="S494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="T494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="U494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="V494" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="W494" s="59" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="495" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H495" s="8"/>
+    <row r="495" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A495" s="57" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B495" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C495" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D495" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E495" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F495" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G495" s="57" t="s">
+        <v>1903</v>
+      </c>
+      <c r="H495" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I495" s="57">
+        <v>111609</v>
+      </c>
+      <c r="J495" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K495" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L495" s="59" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M495" s="57" t="s">
+        <v>1924</v>
+      </c>
+      <c r="N495" s="60">
+        <v>2018</v>
+      </c>
+      <c r="O495" s="59" t="str">
+        <f>O493</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P495" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q495" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R495" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S495" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T495" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U495" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V495" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W495" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="496" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H496" s="8"/>
+      <c r="A496" s="57" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B496" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C496" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D496" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E496" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F496" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G496" s="57" t="s">
+        <v>1905</v>
+      </c>
+      <c r="H496" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I496" s="57">
+        <v>111487</v>
+      </c>
+      <c r="J496" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K496" s="57" t="s">
+        <v>1901</v>
+      </c>
+      <c r="L496" s="59" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M496" s="57" t="s">
+        <v>1925</v>
+      </c>
+      <c r="N496" s="60">
+        <v>2018</v>
+      </c>
+      <c r="O496" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P496" s="57"/>
+      <c r="Q496" s="59"/>
+      <c r="R496" s="62"/>
+      <c r="S496" s="62"/>
+      <c r="T496" s="59"/>
+      <c r="U496" s="59"/>
+      <c r="V496" s="52"/>
+      <c r="W496" s="52"/>
     </row>
-    <row r="497" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H497" s="8"/>
+    <row r="497" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A497" s="57" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B497" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C497" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D497" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E497" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F497" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G497" s="57" t="s">
+        <v>1907</v>
+      </c>
+      <c r="H497" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I497" s="57">
+        <v>111380</v>
+      </c>
+      <c r="J497" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K497" s="57" t="s">
+        <v>1908</v>
+      </c>
+      <c r="L497" s="59" t="s">
+        <v>978</v>
+      </c>
+      <c r="M497" s="57" t="s">
+        <v>1923</v>
+      </c>
+      <c r="N497" s="60">
+        <v>2019</v>
+      </c>
+      <c r="O497" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P497" s="57"/>
+      <c r="Q497" s="59"/>
+      <c r="R497" s="62"/>
+      <c r="S497" s="62"/>
+      <c r="T497" s="59"/>
+      <c r="U497" s="59"/>
+      <c r="V497" s="52"/>
+      <c r="W497" s="52"/>
     </row>
-    <row r="498" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H498" s="8"/>
+    <row r="498" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A498" s="57" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B498" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C498" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D498" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E498" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F498" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G498" s="57" t="s">
+        <v>1910</v>
+      </c>
+      <c r="H498" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I498" s="57">
+        <v>111369</v>
+      </c>
+      <c r="J498" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K498" s="57" t="s">
+        <v>1908</v>
+      </c>
+      <c r="L498" s="59" t="s">
+        <v>978</v>
+      </c>
+      <c r="M498" s="57" t="s">
+        <v>1923</v>
+      </c>
+      <c r="N498" s="60">
+        <v>2018</v>
+      </c>
+      <c r="O498" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P498" s="57"/>
+      <c r="Q498" s="59"/>
+      <c r="R498" s="62"/>
+      <c r="S498" s="62"/>
+      <c r="T498" s="59"/>
+      <c r="U498" s="59"/>
+      <c r="V498" s="52"/>
+      <c r="W498" s="52"/>
     </row>
-    <row r="499" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H499" s="8"/>
+    <row r="499" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A499" s="57" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B499" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C499" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D499" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E499" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F499" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G499" s="57" t="s">
+        <v>1361</v>
+      </c>
+      <c r="H499" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I499" s="57">
+        <v>111362</v>
+      </c>
+      <c r="J499" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K499" s="57" t="s">
+        <v>1912</v>
+      </c>
+      <c r="L499" s="59" t="s">
+        <v>941</v>
+      </c>
+      <c r="M499" s="59" t="s">
+        <v>1913</v>
+      </c>
+      <c r="N499" s="60">
+        <v>1998</v>
+      </c>
+      <c r="O499" s="59" t="s">
+        <v>1914</v>
+      </c>
+      <c r="P499" s="57"/>
+      <c r="Q499" s="59"/>
+      <c r="R499" s="62"/>
+      <c r="S499" s="62"/>
+      <c r="T499" s="59"/>
+      <c r="U499" s="59"/>
+      <c r="V499" s="52"/>
+      <c r="W499" s="52"/>
     </row>
-    <row r="500" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H500" s="8"/>
+    <row r="500" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A500" s="57" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B500" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C500" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D500" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E500" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F500" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G500" s="57" t="s">
+        <v>1916</v>
+      </c>
+      <c r="H500" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I500" s="57">
+        <v>111362</v>
+      </c>
+      <c r="J500" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K500" s="57" t="s">
+        <v>1917</v>
+      </c>
+      <c r="L500" s="59" t="s">
+        <v>1896</v>
+      </c>
+      <c r="M500" s="57" t="s">
+        <v>1921</v>
+      </c>
+      <c r="N500" s="60">
+        <v>2019</v>
+      </c>
+      <c r="O500" s="57" t="s">
+        <v>1918</v>
+      </c>
+      <c r="P500" s="57"/>
+      <c r="Q500" s="59"/>
+      <c r="R500" s="62"/>
+      <c r="S500" s="62"/>
+      <c r="T500" s="59"/>
+      <c r="U500" s="59"/>
+      <c r="V500" s="52"/>
+      <c r="W500" s="52"/>
     </row>
-    <row r="501" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H501" s="8"/>
+    <row r="501" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A501" s="57" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B501" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C501" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D501" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E501" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F501" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G501" s="57" t="s">
+        <v>1920</v>
+      </c>
+      <c r="H501" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I501" s="57">
+        <v>111351</v>
+      </c>
+      <c r="J501" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K501" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L501" s="59" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M501" s="57" t="s">
+        <v>1922</v>
+      </c>
+      <c r="N501" s="60">
+        <v>2015</v>
+      </c>
+      <c r="O501" s="59" t="str">
+        <f>O495</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P501" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q501" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R501" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S501" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T501" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U501" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V501" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W501" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="502" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H502" s="8"/>
+    <row r="502" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A502" s="57" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B502" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C502" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D502" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E502" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F502" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G502" s="57" t="s">
+        <v>1928</v>
+      </c>
+      <c r="H502" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I502" s="66">
+        <v>111315</v>
+      </c>
+      <c r="J502" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K502" s="57" t="s">
+        <v>1929</v>
+      </c>
+      <c r="L502" s="59" t="s">
+        <v>941</v>
+      </c>
+      <c r="M502" s="57" t="s">
+        <v>1913</v>
+      </c>
+      <c r="N502" s="60">
+        <v>2005</v>
+      </c>
+      <c r="O502" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P502" s="57"/>
+      <c r="Q502" s="59"/>
+      <c r="R502" s="62"/>
+      <c r="S502" s="62"/>
+      <c r="T502" s="59"/>
+      <c r="U502" s="59"/>
+      <c r="V502" s="52"/>
+      <c r="W502" s="52"/>
     </row>
-    <row r="503" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H503" s="8"/>
+    <row r="503" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A503" s="57" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B503" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C503" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D503" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E503" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F503" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G503" s="57" t="s">
+        <v>1933</v>
+      </c>
+      <c r="H503" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I503" s="57">
+        <v>111315</v>
+      </c>
+      <c r="J503" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K503" s="57" t="s">
+        <v>1929</v>
+      </c>
+      <c r="L503" s="59" t="s">
+        <v>941</v>
+      </c>
+      <c r="M503" s="57" t="s">
+        <v>1913</v>
+      </c>
+      <c r="N503" s="60">
+        <v>2021</v>
+      </c>
+      <c r="O503" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P503" s="57"/>
+      <c r="Q503" s="59"/>
+      <c r="R503" s="62"/>
+      <c r="S503" s="62"/>
+      <c r="T503" s="59"/>
+      <c r="U503" s="59"/>
+      <c r="V503" s="52"/>
+      <c r="W503" s="52"/>
     </row>
-    <row r="504" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H504" s="8"/>
+    <row r="504" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A504" s="57" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B504" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C504" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D504" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E504" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F504" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G504" s="57" t="s">
+        <v>1932</v>
+      </c>
+      <c r="H504" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I504" s="67">
+        <v>111309</v>
+      </c>
+      <c r="J504" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K504" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L504" s="59" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M504" s="59" t="s">
+        <v>1361</v>
+      </c>
+      <c r="N504" s="60">
+        <v>2011</v>
+      </c>
+      <c r="O504" s="59" t="str">
+        <f>O495</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P504" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q504" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R504" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S504" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T504" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U504" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V504" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W504" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="505" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H505" s="8"/>
+    <row r="505" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A505" s="57" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B505" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C505" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D505" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E505" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F505" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G505" s="57" t="s">
+        <v>583</v>
+      </c>
+      <c r="H505" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I505" s="57">
+        <v>111154</v>
+      </c>
+      <c r="J505" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K505" s="57" t="s">
+        <v>1481</v>
+      </c>
+      <c r="L505" s="59" t="s">
+        <v>951</v>
+      </c>
+      <c r="M505" s="59" t="s">
+        <v>1935</v>
+      </c>
+      <c r="N505" s="60">
+        <v>2007</v>
+      </c>
+      <c r="O505" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P505" s="57"/>
+      <c r="Q505" s="59"/>
+      <c r="R505" s="62"/>
+      <c r="S505" s="62"/>
+      <c r="T505" s="59"/>
+      <c r="U505" s="59"/>
+      <c r="V505" s="52"/>
+      <c r="W505" s="52"/>
     </row>
-    <row r="506" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H506" s="8"/>
+    <row r="506" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A506" s="57" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B506" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C506" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D506" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E506" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F506" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G506" s="57" t="s">
+        <v>1937</v>
+      </c>
+      <c r="H506" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I506" s="57">
+        <v>111138</v>
+      </c>
+      <c r="J506" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K506" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L506" s="59" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M506" s="57" t="s">
+        <v>1882</v>
+      </c>
+      <c r="N506" s="60">
+        <v>2015</v>
+      </c>
+      <c r="O506" s="59" t="str">
+        <f>O504</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P506" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q506" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R506" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S506" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T506" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U506" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V506" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W506" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="507" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H507" s="8"/>
+    <row r="507" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A507" s="57" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B507" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C507" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D507" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E507" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F507" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G507" s="57" t="s">
+        <v>1939</v>
+      </c>
+      <c r="H507" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I507" s="57">
+        <v>111039</v>
+      </c>
+      <c r="J507" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K507" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L507" s="59" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M507" s="57" t="s">
+        <v>1882</v>
+      </c>
+      <c r="N507" s="60">
+        <v>2014</v>
+      </c>
+      <c r="O507" s="59" t="str">
+        <f>O506</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P507" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q507" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R507" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S507" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T507" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U507" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V507" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W507" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="508" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H508" s="8"/>
+    <row r="508" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A508" s="57" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B508" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C508" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D508" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E508" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F508" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G508" s="57" t="s">
+        <v>1941</v>
+      </c>
+      <c r="H508" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I508" s="57">
+        <v>111039</v>
+      </c>
+      <c r="J508" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K508" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L508" s="59" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M508" s="57" t="s">
+        <v>1882</v>
+      </c>
+      <c r="N508" s="60">
+        <v>2014</v>
+      </c>
+      <c r="O508" s="59" t="str">
+        <f>O507</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P508" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q508" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R508" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S508" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T508" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U508" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V508" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W508" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="509" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H509" s="8"/>
+    <row r="509" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A509" s="57" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B509" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C509" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D509" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E509" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F509" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G509" s="57" t="s">
+        <v>1943</v>
+      </c>
+      <c r="H509" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I509" s="57">
+        <v>111014</v>
+      </c>
+      <c r="J509" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K509" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L509" s="59" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M509" s="57" t="s">
+        <v>1944</v>
+      </c>
+      <c r="N509" s="60">
+        <v>2015</v>
+      </c>
+      <c r="O509" s="59" t="str">
+        <f>O508</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P509" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q509" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R509" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S509" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T509" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U509" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V509" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W509" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="510" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H510" s="8"/>
+    <row r="510" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A510" s="57" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B510" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C510" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D510" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E510" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F510" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G510" s="57" t="s">
+        <v>1946</v>
+      </c>
+      <c r="H510" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I510" s="57">
+        <v>110962</v>
+      </c>
+      <c r="J510" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K510" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L510" s="59" t="s">
+        <v>1947</v>
+      </c>
+      <c r="M510" s="57" t="s">
+        <v>1948</v>
+      </c>
+      <c r="N510" s="60">
+        <v>2015</v>
+      </c>
+      <c r="O510" s="59" t="str">
+        <f>O509</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P510" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q510" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R510" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S510" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T510" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U510" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V510" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W510" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="511" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H511" s="8"/>
+    <row r="511" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A511" s="57" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B511" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C511" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D511" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E511" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F511" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G511" s="57" t="s">
+        <v>1950</v>
+      </c>
+      <c r="H511" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I511" s="57" t="s">
+        <v>1951</v>
+      </c>
+      <c r="J511" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K511" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L511" s="59" t="s">
+        <v>1054</v>
+      </c>
+      <c r="M511" s="57" t="s">
+        <v>1952</v>
+      </c>
+      <c r="N511" s="60">
+        <v>2015</v>
+      </c>
+      <c r="O511" s="59" t="str">
+        <f>O510</f>
+        <v>https://doi.org/10.1155/2023/6643006</v>
+      </c>
+      <c r="P511" s="57" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Q511" s="59" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R511" s="62">
+        <v>2023</v>
+      </c>
+      <c r="S511" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="T511" s="59" t="s">
+        <v>1853</v>
+      </c>
+      <c r="U511" s="59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="V511" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W511" s="52" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="512" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H512" s="8"/>
+    <row r="512" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A512" s="57" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B512" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C512" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D512" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E512" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F512" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G512" s="66" t="s">
+        <v>1954</v>
+      </c>
+      <c r="H512" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I512" s="66">
+        <v>110699</v>
+      </c>
+      <c r="J512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K512" s="57" t="s">
+        <v>1955</v>
+      </c>
+      <c r="L512" s="59" t="s">
+        <v>941</v>
+      </c>
+      <c r="M512" s="57" t="s">
+        <v>1956</v>
+      </c>
+      <c r="N512" s="60">
+        <v>2014</v>
+      </c>
+      <c r="O512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="R512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="S512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="T512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="U512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="V512" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="W512" s="59" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="513" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H513" s="8"/>
+    <row r="513" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A513" s="57" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B513" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C513" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D513" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E513" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F513" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G513" s="57" t="s">
+        <v>1958</v>
+      </c>
+      <c r="H513" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I513" s="57">
+        <v>110460</v>
+      </c>
+      <c r="J513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K513" s="57" t="s">
+        <v>1959</v>
+      </c>
+      <c r="L513" s="59" t="s">
+        <v>1452</v>
+      </c>
+      <c r="M513" s="57" t="s">
+        <v>1960</v>
+      </c>
+      <c r="N513" s="60">
+        <v>2022</v>
+      </c>
+      <c r="O513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="R513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="S513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="T513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="U513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="V513" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="W513" s="59" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="514" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H514" s="8"/>
+    <row r="514" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A514" s="57" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B514" s="57" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C514" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D514" s="63" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E514" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F514" s="57" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G514" s="57" t="s">
+        <v>1962</v>
+      </c>
+      <c r="H514" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I514" s="57">
+        <v>110394</v>
+      </c>
+      <c r="J514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K514" s="57" t="s">
+        <v>1881</v>
+      </c>
+      <c r="L514" s="59" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M514" s="57" t="s">
+        <v>1963</v>
+      </c>
+      <c r="N514" s="60">
+        <v>2011</v>
+      </c>
+      <c r="O514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="P514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="R514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="S514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="T514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="U514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="V514" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="W514" s="59" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="515" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H515" s="8"/>
+    <row r="515" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A515" s="57"/>
+      <c r="B515" s="57"/>
+      <c r="C515" s="57"/>
+      <c r="D515" s="63"/>
+      <c r="E515" s="57"/>
+      <c r="F515" s="57"/>
+      <c r="G515" s="57"/>
+      <c r="H515" s="58"/>
+      <c r="I515" s="57"/>
+      <c r="J515" s="59"/>
+      <c r="K515" s="59"/>
+      <c r="L515" s="59"/>
+      <c r="M515" s="59"/>
+      <c r="N515" s="60"/>
+      <c r="O515" s="59"/>
+      <c r="P515" s="57"/>
+      <c r="Q515" s="59"/>
+      <c r="R515" s="62"/>
+      <c r="S515" s="62"/>
+      <c r="T515" s="59"/>
+      <c r="U515" s="59"/>
+      <c r="V515" s="52"/>
+      <c r="W515" s="52"/>
     </row>
-    <row r="516" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H516" s="8"/>
+    <row r="516" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A516" s="52"/>
+      <c r="B516" s="52"/>
+      <c r="C516" s="52"/>
+      <c r="E516" s="52"/>
+      <c r="F516" s="52"/>
+      <c r="G516" s="52"/>
+      <c r="H516" s="53"/>
+      <c r="I516" s="52"/>
+      <c r="J516" s="54"/>
+      <c r="K516" s="54"/>
+      <c r="L516" s="54"/>
+      <c r="M516" s="54"/>
+      <c r="N516" s="55"/>
+      <c r="O516" s="54"/>
+      <c r="P516" s="52"/>
+      <c r="Q516" s="54"/>
+      <c r="R516" s="56"/>
+      <c r="S516" s="56"/>
+      <c r="T516" s="54"/>
+      <c r="U516" s="54"/>
+      <c r="V516" s="52"/>
+      <c r="W516" s="52"/>
     </row>
-    <row r="517" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H517" s="8"/>
+    <row r="517" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A517" s="52"/>
+      <c r="B517" s="52"/>
+      <c r="C517" s="52"/>
+      <c r="E517" s="52"/>
+      <c r="F517" s="52"/>
+      <c r="G517" s="52"/>
+      <c r="H517" s="53"/>
+      <c r="I517" s="52"/>
+      <c r="J517" s="54"/>
+      <c r="K517" s="54"/>
+      <c r="L517" s="54"/>
+      <c r="M517" s="54"/>
+      <c r="N517" s="55"/>
+      <c r="O517" s="54"/>
+      <c r="P517" s="52"/>
+      <c r="Q517" s="54"/>
+      <c r="R517" s="56"/>
+      <c r="S517" s="56"/>
+      <c r="T517" s="54"/>
+      <c r="U517" s="54"/>
+      <c r="V517" s="52"/>
+      <c r="W517" s="52"/>
     </row>
-    <row r="518" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H518" s="8"/>
       <c r="Q518" s="9"/>
     </row>
-    <row r="519" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H519" s="8"/>
     </row>
-    <row r="520" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H520" s="8"/>
       <c r="Q520" s="9"/>
     </row>
-    <row r="521" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H521" s="8"/>
       <c r="Q521" s="9"/>
     </row>
-    <row r="522" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H522" s="8"/>
       <c r="Q522" s="9"/>
     </row>
-    <row r="523" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H523" s="8"/>
       <c r="Q523" s="9"/>
     </row>
-    <row r="524" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H524" s="8"/>
       <c r="Q524" s="9"/>
     </row>
-    <row r="525" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H525" s="8"/>
       <c r="Q525" s="9"/>
     </row>
-    <row r="526" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H526" s="8"/>
       <c r="Q526" s="9"/>
     </row>
-    <row r="527" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H527" s="8"/>
       <c r="Q527" s="9"/>
     </row>
-    <row r="528" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H528" s="8"/>
       <c r="Q528" s="9"/>
     </row>
@@ -74223,9 +76259,11 @@
     <hyperlink ref="R92" r:id="rId51" tooltip="PubMed" display="https://www.ncbi.nlm.nih.gov/pubmed?term=16789247+OR+3959991+OR+2820141+OR+3201750+OR+1549908+OR+1475907+OR+8492091+OR+7698884+OR+8121799+OR+8073636+OR+8021587+OR+9482589+OR+9926400+OR+10456793+OR+11448171" xr:uid="{3FEC8D3C-95EF-49C8-9008-07A50A777F6F}"/>
     <hyperlink ref="O485" r:id="rId52" location=":~:text=Whole-genome%20sequences%20of%20RISV-I%20type%20SBIV-VP13%20and%20RSIV-II" xr:uid="{CD7760A6-BED3-466B-80B4-5C0FB826986C}"/>
     <hyperlink ref="O185" r:id="rId53" display="10.3354/dao03500" xr:uid="{970A3DBD-2CA0-47FF-9146-7327C707266E}"/>
+    <hyperlink ref="O489" r:id="rId54" xr:uid="{D96AE632-AE67-4B78-A05F-EC5474B0845A}"/>
+    <hyperlink ref="O493" r:id="rId55" xr:uid="{98849F9B-2AED-40AB-963C-BFB7A27B5D20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
-  <legacyDrawing r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
+  <legacyDrawing r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uploading file with results of gene tree review
</commit_message>
<xml_diff>
--- a/megalocytivirus_sequence_data.xlsx
+++ b/megalocytivirus_sequence_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{BD7AB48C-5E6D-4A2E-8E66-70A39FE8C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9EBD6B2-7BCC-4772-9DE3-08413AED8459}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{BD7AB48C-5E6D-4A2E-8E66-70A39FE8C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5D417A-A6B1-4D70-BBED-618D6E03D9E4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{CD6C468C-256F-45C2-B81B-3E7578C677C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD6C468C-256F-45C2-B81B-3E7578C677C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Main sheet" sheetId="1" r:id="rId1"/>
@@ -42208,38 +42208,38 @@
   <dimension ref="A1:Y547"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A486" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A488" sqref="A488"/>
+      <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.88671875" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="39.33203125" customWidth="1"/>
-    <col min="6" max="6" width="36.88671875" customWidth="1"/>
-    <col min="7" max="7" width="55.44140625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="47.88671875" customWidth="1"/>
-    <col min="10" max="10" width="29.109375" customWidth="1"/>
-    <col min="11" max="11" width="30.109375" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="26.44140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="44.6640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="46.109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="38.109375" customWidth="1"/>
-    <col min="17" max="17" width="40.44140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="21.44140625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="42.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="83.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" customWidth="1"/>
+    <col min="7" max="7" width="55.42578125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="47.85546875" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="44.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="46.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="38.140625" customWidth="1"/>
+    <col min="17" max="17" width="40.42578125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="42.140625" style="3" customWidth="1"/>
     <col min="20" max="20" width="48" style="2" customWidth="1"/>
-    <col min="21" max="21" width="49.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="49.7109375" style="2" customWidth="1"/>
     <col min="22" max="22" width="48" customWidth="1"/>
-    <col min="23" max="23" width="37.44140625" customWidth="1"/>
-    <col min="24" max="24" width="18.5546875" customWidth="1"/>
+    <col min="23" max="23" width="37.42578125" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>8</v>
       </c>
@@ -42313,7 +42313,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1602</v>
       </c>
@@ -42387,7 +42387,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -42458,7 +42458,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -42532,7 +42532,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>1603</v>
       </c>
@@ -42606,7 +42606,7 @@
         <v>1713</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -42680,7 +42680,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="216" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="240" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -42754,7 +42754,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="216" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="240" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -42826,7 +42826,7 @@
         <v>1709</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -42900,7 +42900,7 @@
         <v>1706</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -42966,7 +42966,7 @@
       </c>
       <c r="W10" s="2"/>
     </row>
-    <row r="11" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>1677</v>
       </c>
@@ -43037,7 +43037,7 @@
         <v>1716</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="216" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>799</v>
       </c>
@@ -43111,7 +43111,7 @@
         <v>1712</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -43176,7 +43176,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -43241,7 +43241,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -43306,7 +43306,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>86</v>
       </c>
@@ -43371,7 +43371,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>87</v>
       </c>
@@ -43436,7 +43436,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -43501,7 +43501,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -43566,7 +43566,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -43631,7 +43631,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -43696,7 +43696,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -43761,7 +43761,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -43826,7 +43826,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -43891,7 +43891,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -43956,7 +43956,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>112</v>
       </c>
@@ -44025,7 +44025,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>115</v>
       </c>
@@ -44094,7 +44094,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>116</v>
       </c>
@@ -44160,7 +44160,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -44225,7 +44225,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="202.2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" ht="225.75" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -44290,7 +44290,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>123</v>
       </c>
@@ -44355,7 +44355,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>147</v>
       </c>
@@ -44426,7 +44426,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1673</v>
       </c>
@@ -44492,7 +44492,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>150</v>
       </c>
@@ -44551,7 +44551,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>156</v>
       </c>
@@ -44616,7 +44616,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>154</v>
       </c>
@@ -44681,7 +44681,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>158</v>
       </c>
@@ -44746,7 +44746,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>191</v>
       </c>
@@ -44805,7 +44805,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -44870,7 +44870,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -44935,7 +44935,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>175</v>
       </c>
@@ -45000,7 +45000,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>178</v>
       </c>
@@ -45065,7 +45065,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>179</v>
       </c>
@@ -45130,7 +45130,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>181</v>
       </c>
@@ -45195,7 +45195,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>182</v>
       </c>
@@ -45260,7 +45260,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -45325,7 +45325,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>184</v>
       </c>
@@ -45390,7 +45390,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -45455,7 +45455,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>190</v>
       </c>
@@ -45520,7 +45520,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>195</v>
       </c>
@@ -45585,7 +45585,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>197</v>
       </c>
@@ -45650,7 +45650,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>199</v>
       </c>
@@ -45715,7 +45715,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>202</v>
       </c>
@@ -45780,7 +45780,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -45845,7 +45845,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>208</v>
       </c>
@@ -45910,7 +45910,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" ht="225" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>211</v>
       </c>
@@ -45975,7 +45975,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" ht="225" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>216</v>
       </c>
@@ -46038,7 +46038,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>218</v>
       </c>
@@ -46103,7 +46103,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>223</v>
       </c>
@@ -46168,7 +46168,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>225</v>
       </c>
@@ -46233,7 +46233,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="61" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>227</v>
       </c>
@@ -46298,7 +46298,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="62" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>229</v>
       </c>
@@ -46363,7 +46363,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>233</v>
       </c>
@@ -46428,7 +46428,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="64" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>236</v>
       </c>
@@ -46493,7 +46493,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>237</v>
       </c>
@@ -46558,7 +46558,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>239</v>
       </c>
@@ -46623,7 +46623,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>240</v>
       </c>
@@ -46688,7 +46688,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>242</v>
       </c>
@@ -46753,7 +46753,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>243</v>
       </c>
@@ -46818,7 +46818,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>244</v>
       </c>
@@ -46883,7 +46883,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>246</v>
       </c>
@@ -46948,7 +46948,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>247</v>
       </c>
@@ -47013,7 +47013,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>248</v>
       </c>
@@ -47078,7 +47078,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" ht="270" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>250</v>
       </c>
@@ -47143,7 +47143,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" ht="270" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>258</v>
       </c>
@@ -47208,7 +47208,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="76" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>261</v>
       </c>
@@ -47274,7 +47274,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="77" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" ht="180" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>265</v>
       </c>
@@ -47340,7 +47340,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" ht="180" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>273</v>
       </c>
@@ -47406,7 +47406,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" ht="180" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>285</v>
       </c>
@@ -47472,7 +47472,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" ht="180" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>286</v>
       </c>
@@ -47538,7 +47538,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>287</v>
       </c>
@@ -47604,7 +47604,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>288</v>
       </c>
@@ -47670,7 +47670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>289</v>
       </c>
@@ -47736,7 +47736,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>290</v>
       </c>
@@ -47802,7 +47802,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>291</v>
       </c>
@@ -47868,7 +47868,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>292</v>
       </c>
@@ -47934,7 +47934,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>293</v>
       </c>
@@ -48000,7 +48000,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>294</v>
       </c>
@@ -48066,7 +48066,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>295</v>
       </c>
@@ -48132,7 +48132,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:24" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:24" ht="300" x14ac:dyDescent="0.25">
       <c r="A90" s="35" t="s">
         <v>1604</v>
       </c>
@@ -48206,7 +48206,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="91" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>21</v>
       </c>
@@ -48280,7 +48280,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="92" spans="1:24" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A92" s="35" t="s">
         <v>1599</v>
       </c>
@@ -48352,7 +48352,7 @@
         <v>1702</v>
       </c>
     </row>
-    <row r="93" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>307</v>
       </c>
@@ -48418,7 +48418,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="94" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>308</v>
       </c>
@@ -48484,7 +48484,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="95" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="35" t="s">
         <v>1610</v>
       </c>
@@ -48558,7 +48558,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="96" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>315</v>
       </c>
@@ -48624,7 +48624,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="97" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>319</v>
       </c>
@@ -48690,7 +48690,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:24" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
         <v>1576</v>
       </c>
@@ -48756,7 +48756,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="99" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>326</v>
       </c>
@@ -48822,7 +48822,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="100" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>327</v>
       </c>
@@ -48888,7 +48888,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="101" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>331</v>
       </c>
@@ -48954,7 +48954,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="102" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>335</v>
       </c>
@@ -49020,7 +49020,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="103" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>340</v>
       </c>
@@ -49086,7 +49086,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="104" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>341</v>
       </c>
@@ -49152,7 +49152,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="105" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>342</v>
       </c>
@@ -49218,7 +49218,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="106" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>349</v>
       </c>
@@ -49284,7 +49284,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="107" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>350</v>
       </c>
@@ -49350,7 +49350,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="108" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>351</v>
       </c>
@@ -49416,7 +49416,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="109" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>352</v>
       </c>
@@ -49482,7 +49482,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="110" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>353</v>
       </c>
@@ -49548,7 +49548,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="111" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>354</v>
       </c>
@@ -49614,7 +49614,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="112" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>361</v>
       </c>
@@ -49680,7 +49680,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="113" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>365</v>
       </c>
@@ -49746,7 +49746,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="114" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>368</v>
       </c>
@@ -49812,7 +49812,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="115" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>374</v>
       </c>
@@ -49878,7 +49878,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="116" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>376</v>
       </c>
@@ -49944,7 +49944,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="117" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>377</v>
       </c>
@@ -50010,7 +50010,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="118" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>379</v>
       </c>
@@ -50076,7 +50076,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="119" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>380</v>
       </c>
@@ -50142,7 +50142,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="120" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>381</v>
       </c>
@@ -50208,7 +50208,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>382</v>
       </c>
@@ -50274,7 +50274,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="122" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>383</v>
       </c>
@@ -50336,7 +50336,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="123" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>1230</v>
       </c>
@@ -50410,7 +50410,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="124" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>1235</v>
       </c>
@@ -50484,7 +50484,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="125" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>404</v>
       </c>
@@ -50550,7 +50550,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="126" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>1434</v>
       </c>
@@ -50619,7 +50619,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="127" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>408</v>
       </c>
@@ -50685,7 +50685,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="128" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>410</v>
       </c>
@@ -50751,7 +50751,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="129" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>412</v>
       </c>
@@ -50817,7 +50817,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="130" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>414</v>
       </c>
@@ -50883,7 +50883,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="131" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>416</v>
       </c>
@@ -50949,7 +50949,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="132" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>418</v>
       </c>
@@ -51015,7 +51015,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="133" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>41</v>
       </c>
@@ -51086,7 +51086,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>398</v>
       </c>
@@ -51160,7 +51160,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="135" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>400</v>
       </c>
@@ -51234,7 +51234,7 @@
         <v>1721</v>
       </c>
     </row>
-    <row r="136" spans="1:24" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>61</v>
       </c>
@@ -51308,7 +51308,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="137" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>428</v>
       </c>
@@ -51374,7 +51374,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="138" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>430</v>
       </c>
@@ -51440,7 +51440,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="139" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>432</v>
       </c>
@@ -51506,7 +51506,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="140" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>434</v>
       </c>
@@ -51572,7 +51572,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="141" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>436</v>
       </c>
@@ -51638,7 +51638,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="142" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>438</v>
       </c>
@@ -51704,7 +51704,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="143" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>440</v>
       </c>
@@ -51770,7 +51770,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="144" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>442</v>
       </c>
@@ -51836,7 +51836,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="145" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>444</v>
       </c>
@@ -51902,7 +51902,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="146" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>446</v>
       </c>
@@ -51968,7 +51968,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="147" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>448</v>
       </c>
@@ -52034,7 +52034,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="148" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>450</v>
       </c>
@@ -52100,7 +52100,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="149" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>452</v>
       </c>
@@ -52166,7 +52166,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="150" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>454</v>
       </c>
@@ -52232,7 +52232,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="151" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>456</v>
       </c>
@@ -52298,7 +52298,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="152" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>457</v>
       </c>
@@ -52364,7 +52364,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="153" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>458</v>
       </c>
@@ -52430,7 +52430,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="154" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>459</v>
       </c>
@@ -52496,7 +52496,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="155" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>460</v>
       </c>
@@ -52562,7 +52562,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="156" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>461</v>
       </c>
@@ -52628,7 +52628,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="157" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>462</v>
       </c>
@@ -52694,7 +52694,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="158" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>463</v>
       </c>
@@ -52760,7 +52760,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="159" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>464</v>
       </c>
@@ -52826,7 +52826,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="160" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>465</v>
       </c>
@@ -52892,7 +52892,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>466</v>
       </c>
@@ -52958,7 +52958,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="162" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>467</v>
       </c>
@@ -53024,7 +53024,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="163" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>468</v>
       </c>
@@ -53090,7 +53090,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="164" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>469</v>
       </c>
@@ -53156,7 +53156,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="165" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>470</v>
       </c>
@@ -53222,7 +53222,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="166" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>471</v>
       </c>
@@ -53288,7 +53288,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="167" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>472</v>
       </c>
@@ -53354,7 +53354,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>473</v>
       </c>
@@ -53420,7 +53420,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="169" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>474</v>
       </c>
@@ -53486,7 +53486,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="170" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>475</v>
       </c>
@@ -53552,7 +53552,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>476</v>
       </c>
@@ -53618,7 +53618,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="172" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>477</v>
       </c>
@@ -53684,7 +53684,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="173" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>478</v>
       </c>
@@ -53750,7 +53750,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="174" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>479</v>
       </c>
@@ -53816,7 +53816,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="175" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>480</v>
       </c>
@@ -53882,7 +53882,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="176" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>481</v>
       </c>
@@ -53948,7 +53948,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="177" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>482</v>
       </c>
@@ -54014,7 +54014,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="178" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>483</v>
       </c>
@@ -54080,7 +54080,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="179" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>484</v>
       </c>
@@ -54146,7 +54146,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="180" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>486</v>
       </c>
@@ -54212,7 +54212,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="181" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>487</v>
       </c>
@@ -54278,7 +54278,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="182" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>488</v>
       </c>
@@ -54344,7 +54344,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="183" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>489</v>
       </c>
@@ -54410,7 +54410,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="184" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>491</v>
       </c>
@@ -54476,7 +54476,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="185" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>66</v>
       </c>
@@ -54550,7 +54550,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="186" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>493</v>
       </c>
@@ -54616,7 +54616,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="187" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>495</v>
       </c>
@@ -54678,7 +54678,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="188" spans="1:24" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>496</v>
       </c>
@@ -54742,7 +54742,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="189" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>497</v>
       </c>
@@ -54808,7 +54808,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="190" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>498</v>
       </c>
@@ -54865,7 +54865,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="191" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>499</v>
       </c>
@@ -54922,7 +54922,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="192" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>500</v>
       </c>
@@ -54979,7 +54979,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="193" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>501</v>
       </c>
@@ -55036,7 +55036,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="194" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>502</v>
       </c>
@@ -55093,7 +55093,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="195" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>503</v>
       </c>
@@ -55150,7 +55150,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="196" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>504</v>
       </c>
@@ -55207,7 +55207,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="197" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>505</v>
       </c>
@@ -55264,7 +55264,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="198" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>506</v>
       </c>
@@ -55330,7 +55330,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="199" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>507</v>
       </c>
@@ -55396,7 +55396,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="200" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>509</v>
       </c>
@@ -55462,7 +55462,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="201" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>511</v>
       </c>
@@ -55525,7 +55525,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="202" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>512</v>
       </c>
@@ -55591,7 +55591,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="203" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>514</v>
       </c>
@@ -55657,7 +55657,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="204" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>515</v>
       </c>
@@ -55723,7 +55723,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="205" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>516</v>
       </c>
@@ -55789,7 +55789,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="206" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>518</v>
       </c>
@@ -55855,7 +55855,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="207" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>519</v>
       </c>
@@ -55921,7 +55921,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="208" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>520</v>
       </c>
@@ -55987,7 +55987,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="209" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>522</v>
       </c>
@@ -56053,7 +56053,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="210" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>523</v>
       </c>
@@ -56119,7 +56119,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="211" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>524</v>
       </c>
@@ -56185,7 +56185,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="212" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>526</v>
       </c>
@@ -56251,7 +56251,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="213" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>527</v>
       </c>
@@ -56317,7 +56317,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="214" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>528</v>
       </c>
@@ -56383,7 +56383,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="215" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>530</v>
       </c>
@@ -56449,7 +56449,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="216" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>531</v>
       </c>
@@ -56515,7 +56515,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="217" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>532</v>
       </c>
@@ -56581,7 +56581,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="218" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>534</v>
       </c>
@@ -56647,7 +56647,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="219" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>535</v>
       </c>
@@ -56713,7 +56713,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="220" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>536</v>
       </c>
@@ -56779,7 +56779,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="221" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>538</v>
       </c>
@@ -56845,7 +56845,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="222" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>539</v>
       </c>
@@ -56911,7 +56911,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="223" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>540</v>
       </c>
@@ -56977,7 +56977,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="224" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>542</v>
       </c>
@@ -57043,7 +57043,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="225" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>543</v>
       </c>
@@ -57106,7 +57106,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="226" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>544</v>
       </c>
@@ -57171,7 +57171,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="227" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>545</v>
       </c>
@@ -57236,7 +57236,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="228" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>546</v>
       </c>
@@ -57301,7 +57301,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="229" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>547</v>
       </c>
@@ -57366,7 +57366,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="230" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>548</v>
       </c>
@@ -57431,7 +57431,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="231" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>549</v>
       </c>
@@ -57496,7 +57496,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="232" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>550</v>
       </c>
@@ -57561,7 +57561,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="233" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>551</v>
       </c>
@@ -57626,7 +57626,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="234" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:22" ht="120" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>552</v>
       </c>
@@ -57691,7 +57691,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="235" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>553</v>
       </c>
@@ -57756,7 +57756,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="236" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>554</v>
       </c>
@@ -57821,7 +57821,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="237" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:22" ht="120" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>555</v>
       </c>
@@ -57886,7 +57886,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="238" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>556</v>
       </c>
@@ -57951,7 +57951,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="239" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>557</v>
       </c>
@@ -58016,7 +58016,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="240" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>558</v>
       </c>
@@ -58081,7 +58081,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="241" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>559</v>
       </c>
@@ -58146,7 +58146,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="242" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>560</v>
       </c>
@@ -58211,7 +58211,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="243" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>561</v>
       </c>
@@ -58276,7 +58276,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="244" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>562</v>
       </c>
@@ -58339,7 +58339,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="245" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>563</v>
       </c>
@@ -58404,7 +58404,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="246" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>564</v>
       </c>
@@ -58469,7 +58469,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="247" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>565</v>
       </c>
@@ -58534,7 +58534,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="248" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>566</v>
       </c>
@@ -58599,7 +58599,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="249" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>567</v>
       </c>
@@ -58664,7 +58664,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="250" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:22" ht="120" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>568</v>
       </c>
@@ -58729,7 +58729,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="251" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>569</v>
       </c>
@@ -58794,7 +58794,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="252" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>570</v>
       </c>
@@ -58859,7 +58859,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="253" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>571</v>
       </c>
@@ -58924,7 +58924,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="254" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>572</v>
       </c>
@@ -58989,7 +58989,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="255" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>573</v>
       </c>
@@ -59054,7 +59054,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="256" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>574</v>
       </c>
@@ -59119,7 +59119,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="257" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>575</v>
       </c>
@@ -59184,7 +59184,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="258" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>576</v>
       </c>
@@ -59249,7 +59249,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="259" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>577</v>
       </c>
@@ -59314,7 +59314,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="260" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>578</v>
       </c>
@@ -59379,7 +59379,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="261" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>579</v>
       </c>
@@ -59444,7 +59444,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="262" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>580</v>
       </c>
@@ -59509,7 +59509,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="263" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>581</v>
       </c>
@@ -59574,7 +59574,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="264" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>583</v>
       </c>
@@ -59643,7 +59643,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="265" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>584</v>
       </c>
@@ -59712,7 +59712,7 @@
         <v>1708</v>
       </c>
     </row>
-    <row r="266" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>585</v>
       </c>
@@ -59778,7 +59778,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="267" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>586</v>
       </c>
@@ -59844,7 +59844,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="268" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>587</v>
       </c>
@@ -59910,7 +59910,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="269" spans="1:24" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:24" ht="285" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>588</v>
       </c>
@@ -59976,7 +59976,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="270" spans="1:24" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:24" ht="285" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>589</v>
       </c>
@@ -60042,7 +60042,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="271" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>590</v>
       </c>
@@ -60108,7 +60108,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="272" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>591</v>
       </c>
@@ -60174,7 +60174,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="273" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>592</v>
       </c>
@@ -60240,7 +60240,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="274" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>593</v>
       </c>
@@ -60306,7 +60306,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="275" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>594</v>
       </c>
@@ -60372,7 +60372,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="276" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>595</v>
       </c>
@@ -60441,7 +60441,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="277" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>596</v>
       </c>
@@ -60507,7 +60507,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="278" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>597</v>
       </c>
@@ -60573,7 +60573,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="279" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>598</v>
       </c>
@@ -60639,7 +60639,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="280" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>599</v>
       </c>
@@ -60705,7 +60705,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="281" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>600</v>
       </c>
@@ -60771,7 +60771,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="282" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>601</v>
       </c>
@@ -60840,7 +60840,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="283" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>602</v>
       </c>
@@ -60909,7 +60909,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="284" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>603</v>
       </c>
@@ -60978,7 +60978,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="285" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>604</v>
       </c>
@@ -61047,7 +61047,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="286" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>797</v>
       </c>
@@ -61113,7 +61113,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="287" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>1043</v>
       </c>
@@ -61184,7 +61184,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="288" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>801</v>
       </c>
@@ -61250,7 +61250,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="289" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>802</v>
       </c>
@@ -61316,7 +61316,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="290" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>803</v>
       </c>
@@ -61382,7 +61382,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="291" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>804</v>
       </c>
@@ -61448,7 +61448,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="292" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>805</v>
       </c>
@@ -61514,7 +61514,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="293" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>806</v>
       </c>
@@ -61579,7 +61579,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="294" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>808</v>
       </c>
@@ -61645,7 +61645,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="295" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:22" ht="120" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>809</v>
       </c>
@@ -61711,7 +61711,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="296" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:22" ht="120" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>810</v>
       </c>
@@ -61777,7 +61777,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="297" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:22" ht="150" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>811</v>
       </c>
@@ -61842,7 +61842,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="298" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:22" ht="120" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>812</v>
       </c>
@@ -61908,7 +61908,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="299" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:22" ht="180" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>813</v>
       </c>
@@ -61973,7 +61973,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="300" spans="1:22" ht="144" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:22" ht="165" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>815</v>
       </c>
@@ -62038,7 +62038,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="301" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>817</v>
       </c>
@@ -62103,7 +62103,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="302" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>819</v>
       </c>
@@ -62168,7 +62168,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="303" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>821</v>
       </c>
@@ -62233,7 +62233,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="304" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>823</v>
       </c>
@@ -62298,7 +62298,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="305" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>825</v>
       </c>
@@ -62363,7 +62363,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="306" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>827</v>
       </c>
@@ -62428,7 +62428,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="307" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>829</v>
       </c>
@@ -62493,7 +62493,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="308" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>831</v>
       </c>
@@ -62558,7 +62558,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="309" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>833</v>
       </c>
@@ -62623,7 +62623,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="310" spans="1:25" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:25" ht="225" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>870</v>
       </c>
@@ -62690,7 +62690,7 @@
       <c r="X310" s="2"/>
       <c r="Y310" s="2"/>
     </row>
-    <row r="311" spans="1:25" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:25" ht="225" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>872</v>
       </c>
@@ -62759,7 +62759,7 @@
       </c>
       <c r="X311" s="2"/>
     </row>
-    <row r="312" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:25" ht="120" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>873</v>
       </c>
@@ -62825,7 +62825,7 @@
       </c>
       <c r="X312" s="2"/>
     </row>
-    <row r="313" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:25" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>874</v>
       </c>
@@ -62891,7 +62891,7 @@
       </c>
       <c r="X313" s="2"/>
     </row>
-    <row r="314" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:25" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>875</v>
       </c>
@@ -62955,7 +62955,7 @@
       </c>
       <c r="X314" s="2"/>
     </row>
-    <row r="315" spans="1:25" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:25" ht="105" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>876</v>
       </c>
@@ -63019,7 +63019,7 @@
       </c>
       <c r="X315" s="2"/>
     </row>
-    <row r="316" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>877</v>
       </c>
@@ -63085,7 +63085,7 @@
       </c>
       <c r="X316" s="2"/>
     </row>
-    <row r="317" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:25" ht="90" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>878</v>
       </c>
@@ -63152,7 +63152,7 @@
       <c r="X317" s="2"/>
       <c r="Y317" s="2"/>
     </row>
-    <row r="318" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:25" ht="120" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>880</v>
       </c>
@@ -63219,7 +63219,7 @@
       <c r="X318" s="2"/>
       <c r="Y318" s="2"/>
     </row>
-    <row r="319" spans="1:25" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:25" ht="120" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>883</v>
       </c>
@@ -63283,7 +63283,7 @@
       </c>
       <c r="X319" s="2"/>
     </row>
-    <row r="320" spans="1:25" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:25" ht="105" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>884</v>
       </c>
@@ -63350,7 +63350,7 @@
       <c r="X320" s="2"/>
       <c r="Y320" s="2"/>
     </row>
-    <row r="321" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>1685</v>
       </c>
@@ -63421,7 +63421,7 @@
         <v>1726</v>
       </c>
     </row>
-    <row r="322" spans="1:24" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:24" ht="285" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>889</v>
       </c>
@@ -63487,7 +63487,7 @@
       </c>
       <c r="X322" s="2"/>
     </row>
-    <row r="323" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>891</v>
       </c>
@@ -63553,7 +63553,7 @@
       </c>
       <c r="X323" s="2"/>
     </row>
-    <row r="324" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>892</v>
       </c>
@@ -63619,7 +63619,7 @@
       </c>
       <c r="X324" s="2"/>
     </row>
-    <row r="325" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>918</v>
       </c>
@@ -63685,7 +63685,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="326" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>920</v>
       </c>
@@ -63751,7 +63751,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="327" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>921</v>
       </c>
@@ -63817,7 +63817,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="328" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A328" s="18" t="s">
         <v>1962</v>
       </c>
@@ -63886,7 +63886,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="329" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A329" s="18" t="s">
         <v>1963</v>
       </c>
@@ -63957,7 +63957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="330" spans="1:24" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:24" ht="300" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>928</v>
       </c>
@@ -64022,7 +64022,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="331" spans="1:24" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:24" ht="300" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>930</v>
       </c>
@@ -64087,7 +64087,7 @@
         <v>1832</v>
       </c>
     </row>
-    <row r="332" spans="1:24" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:24" ht="300" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>931</v>
       </c>
@@ -64152,7 +64152,7 @@
         <v>1833</v>
       </c>
     </row>
-    <row r="333" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>936</v>
       </c>
@@ -64217,7 +64217,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="334" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>943</v>
       </c>
@@ -64281,7 +64281,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="335" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>946</v>
       </c>
@@ -64347,7 +64347,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="336" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>952</v>
       </c>
@@ -64413,7 +64413,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="337" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>954</v>
       </c>
@@ -64479,7 +64479,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="338" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>956</v>
       </c>
@@ -64545,7 +64545,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="339" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>958</v>
       </c>
@@ -64611,7 +64611,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="340" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>960</v>
       </c>
@@ -64677,7 +64677,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="341" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>962</v>
       </c>
@@ -64743,7 +64743,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="342" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>964</v>
       </c>
@@ -64809,7 +64809,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="343" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>966</v>
       </c>
@@ -64875,7 +64875,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="344" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>968</v>
       </c>
@@ -64941,7 +64941,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="345" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>970</v>
       </c>
@@ -65007,7 +65007,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="346" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>972</v>
       </c>
@@ -65073,7 +65073,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="347" spans="1:22" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>974</v>
       </c>
@@ -65138,7 +65138,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="348" spans="1:22" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>979</v>
       </c>
@@ -65203,7 +65203,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="349" spans="1:22" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>983</v>
       </c>
@@ -65268,7 +65268,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="350" spans="1:22" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>987</v>
       </c>
@@ -65333,7 +65333,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="351" spans="1:22" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>988</v>
       </c>
@@ -65398,7 +65398,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="352" spans="1:22" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>989</v>
       </c>
@@ -65463,7 +65463,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="353" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>990</v>
       </c>
@@ -65528,7 +65528,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="354" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>992</v>
       </c>
@@ -65593,7 +65593,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="355" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>1039</v>
       </c>
@@ -65664,7 +65664,7 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="356" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>1017</v>
       </c>
@@ -65730,7 +65730,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="357" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>1021</v>
       </c>
@@ -65796,7 +65796,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="358" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A358" s="8" t="s">
         <v>1022</v>
       </c>
@@ -65862,7 +65862,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="359" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>1027</v>
       </c>
@@ -65929,7 +65929,7 @@
       </c>
       <c r="W359" s="2"/>
     </row>
-    <row r="360" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>1030</v>
       </c>
@@ -65995,7 +65995,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="361" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>1033</v>
       </c>
@@ -66061,7 +66061,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="362" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>492</v>
       </c>
@@ -66132,7 +66132,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="363" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>887</v>
       </c>
@@ -66203,7 +66203,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="364" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>312</v>
       </c>
@@ -66274,7 +66274,7 @@
         <v>1731</v>
       </c>
     </row>
-    <row r="365" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>1046</v>
       </c>
@@ -66340,7 +66340,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="366" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>1049</v>
       </c>
@@ -66406,7 +66406,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="367" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>1050</v>
       </c>
@@ -66472,7 +66472,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="368" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>1054</v>
       </c>
@@ -66538,7 +66538,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="369" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>1056</v>
       </c>
@@ -66604,7 +66604,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="370" spans="1:24" ht="288" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:24" ht="315" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>1058</v>
       </c>
@@ -66669,7 +66669,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="371" spans="1:24" ht="288" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:24" ht="315" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>1061</v>
       </c>
@@ -66734,7 +66734,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="372" spans="1:24" ht="288" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:24" ht="315" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>1063</v>
       </c>
@@ -66799,7 +66799,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="373" spans="1:24" ht="288" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:24" ht="315" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>1065</v>
       </c>
@@ -66864,7 +66864,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="374" spans="1:24" ht="288" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:24" ht="315" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>1066</v>
       </c>
@@ -66929,7 +66929,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="375" spans="1:24" ht="288" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:24" ht="315" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>1067</v>
       </c>
@@ -66994,7 +66994,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="376" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>1095</v>
       </c>
@@ -67059,7 +67059,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="377" spans="1:24" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:24" ht="315" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>1581</v>
       </c>
@@ -67130,7 +67130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="378" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>1104</v>
       </c>
@@ -67195,7 +67195,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="379" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>1110</v>
       </c>
@@ -67260,7 +67260,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="380" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>1068</v>
       </c>
@@ -67331,7 +67331,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="381" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>1117</v>
       </c>
@@ -67396,7 +67396,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="382" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>1123</v>
       </c>
@@ -67461,7 +67461,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="383" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>1125</v>
       </c>
@@ -67526,7 +67526,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="384" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>1129</v>
       </c>
@@ -67591,7 +67591,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="385" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>1133</v>
       </c>
@@ -67656,7 +67656,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="386" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>1134</v>
       </c>
@@ -67721,7 +67721,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="387" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>1136</v>
       </c>
@@ -67786,7 +67786,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="388" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>1138</v>
       </c>
@@ -67851,7 +67851,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="389" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>1139</v>
       </c>
@@ -67916,7 +67916,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="390" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>1144</v>
       </c>
@@ -67981,7 +67981,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="391" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>1145</v>
       </c>
@@ -68046,7 +68046,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="392" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>1146</v>
       </c>
@@ -68111,7 +68111,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="393" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>1148</v>
       </c>
@@ -68176,7 +68176,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="394" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>1149</v>
       </c>
@@ -68241,7 +68241,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="395" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>1150</v>
       </c>
@@ -68306,7 +68306,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="396" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>1152</v>
       </c>
@@ -68371,7 +68371,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="397" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:22" ht="165" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>1153</v>
       </c>
@@ -68436,7 +68436,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="398" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>1155</v>
       </c>
@@ -68501,7 +68501,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="399" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>1156</v>
       </c>
@@ -68566,7 +68566,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="400" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>1157</v>
       </c>
@@ -68631,7 +68631,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="401" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>1158</v>
       </c>
@@ -68696,7 +68696,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="402" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>1159</v>
       </c>
@@ -68761,7 +68761,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="403" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>1160</v>
       </c>
@@ -68826,7 +68826,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="404" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>1161</v>
       </c>
@@ -68891,7 +68891,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="405" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>1162</v>
       </c>
@@ -68956,7 +68956,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="406" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>1163</v>
       </c>
@@ -69019,7 +69019,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="407" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>1168</v>
       </c>
@@ -69084,7 +69084,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="408" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>1173</v>
       </c>
@@ -69149,7 +69149,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="409" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>1175</v>
       </c>
@@ -69214,7 +69214,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="410" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>1178</v>
       </c>
@@ -69279,7 +69279,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="411" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>1180</v>
       </c>
@@ -69344,7 +69344,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="412" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>1183</v>
       </c>
@@ -69409,7 +69409,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="413" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>1186</v>
       </c>
@@ -69474,7 +69474,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="414" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>1188</v>
       </c>
@@ -69539,7 +69539,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="415" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>1191</v>
       </c>
@@ -69604,7 +69604,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="416" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>1193</v>
       </c>
@@ -69669,7 +69669,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="417" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>1195</v>
       </c>
@@ -69734,7 +69734,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="418" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>1198</v>
       </c>
@@ -69799,7 +69799,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="419" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>1201</v>
       </c>
@@ -69864,7 +69864,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="420" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>1203</v>
       </c>
@@ -69929,7 +69929,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="421" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>1206</v>
       </c>
@@ -69994,7 +69994,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="422" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>1208</v>
       </c>
@@ -70059,7 +70059,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="423" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>1209</v>
       </c>
@@ -70124,7 +70124,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="424" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>1210</v>
       </c>
@@ -70189,7 +70189,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="425" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>1211</v>
       </c>
@@ -70254,7 +70254,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="426" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>1212</v>
       </c>
@@ -70319,7 +70319,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="427" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>1213</v>
       </c>
@@ -70384,7 +70384,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="428" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>1214</v>
       </c>
@@ -70449,7 +70449,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="429" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>1215</v>
       </c>
@@ -70514,7 +70514,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="430" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>1216</v>
       </c>
@@ -70579,7 +70579,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="431" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>1217</v>
       </c>
@@ -70644,7 +70644,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="432" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>1218</v>
       </c>
@@ -70709,7 +70709,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="433" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>1219</v>
       </c>
@@ -70774,7 +70774,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="434" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>1220</v>
       </c>
@@ -70839,7 +70839,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="435" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>1221</v>
       </c>
@@ -70904,7 +70904,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="436" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>1222</v>
       </c>
@@ -70969,7 +70969,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="437" spans="1:24" ht="288" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:24" ht="330" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>1223</v>
       </c>
@@ -71035,7 +71035,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="438" spans="1:24" ht="288" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:24" ht="330" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>1229</v>
       </c>
@@ -71101,7 +71101,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="439" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>424</v>
       </c>
@@ -71172,7 +71172,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="440" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>426</v>
       </c>
@@ -71243,7 +71243,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="441" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>1239</v>
       </c>
@@ -71309,7 +71309,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="442" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>1243</v>
       </c>
@@ -71375,7 +71375,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="443" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>1247</v>
       </c>
@@ -71441,7 +71441,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="444" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>1250</v>
       </c>
@@ -71507,7 +71507,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="445" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>1251</v>
       </c>
@@ -71573,7 +71573,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="446" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>1252</v>
       </c>
@@ -71639,7 +71639,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="447" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>1253</v>
       </c>
@@ -71705,7 +71705,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="448" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>1254</v>
       </c>
@@ -71771,7 +71771,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="449" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>1255</v>
       </c>
@@ -71837,7 +71837,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="450" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>1256</v>
       </c>
@@ -71903,7 +71903,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="451" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>1257</v>
       </c>
@@ -71969,7 +71969,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="452" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>1258</v>
       </c>
@@ -72035,7 +72035,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="453" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>1259</v>
       </c>
@@ -72101,7 +72101,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="454" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>1260</v>
       </c>
@@ -72167,7 +72167,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="455" spans="1:22" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>1261</v>
       </c>
@@ -72233,7 +72233,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="456" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>1267</v>
       </c>
@@ -72299,7 +72299,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="457" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>1272</v>
       </c>
@@ -72365,7 +72365,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="458" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>1276</v>
       </c>
@@ -72431,7 +72431,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="459" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>1277</v>
       </c>
@@ -72497,7 +72497,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="460" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>1279</v>
       </c>
@@ -72563,7 +72563,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="461" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>1280</v>
       </c>
@@ -72629,7 +72629,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="462" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>1281</v>
       </c>
@@ -72695,7 +72695,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="463" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>1282</v>
       </c>
@@ -72761,7 +72761,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="464" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>1283</v>
       </c>
@@ -72827,7 +72827,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="465" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>1285</v>
       </c>
@@ -72893,7 +72893,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="466" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>1287</v>
       </c>
@@ -72959,7 +72959,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="467" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>1288</v>
       </c>
@@ -73025,7 +73025,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="468" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>1111</v>
       </c>
@@ -73096,7 +73096,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="469" spans="1:24" ht="216" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A469" s="35" t="s">
         <v>1593</v>
       </c>
@@ -73164,7 +73164,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="470" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A470" s="35" t="s">
         <v>1594</v>
       </c>
@@ -73226,7 +73226,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="471" spans="1:24" ht="360" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A471" s="35" t="s">
         <v>1595</v>
       </c>
@@ -73294,7 +73294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="472" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A472" s="35" t="s">
         <v>1596</v>
       </c>
@@ -73363,7 +73363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="473" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A473" s="35" t="s">
         <v>1597</v>
       </c>
@@ -73431,7 +73431,7 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="474" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>280</v>
       </c>
@@ -73502,7 +73502,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="475" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>1359</v>
       </c>
@@ -73571,7 +73571,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="476" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>1539</v>
       </c>
@@ -73630,7 +73630,7 @@
         <v>1543</v>
       </c>
     </row>
-    <row r="477" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>281</v>
       </c>
@@ -73701,7 +73701,7 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="478" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A478" s="35" t="s">
         <v>1577</v>
       </c>
@@ -73772,7 +73772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="479" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A479" s="35" t="s">
         <v>1598</v>
       </c>
@@ -73840,7 +73840,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="480" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>305</v>
       </c>
@@ -73914,7 +73914,7 @@
         <v>1739</v>
       </c>
     </row>
-    <row r="481" spans="1:24" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:24" ht="255" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>1035</v>
       </c>
@@ -73985,7 +73985,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="482" spans="1:24" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A482" s="35" t="s">
         <v>1600</v>
       </c>
@@ -74054,7 +74054,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="483" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A483" s="35" t="s">
         <v>1601</v>
       </c>
@@ -74125,7 +74125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="484" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>56</v>
       </c>
@@ -74190,7 +74190,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="485" spans="1:24" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A485" s="10" t="s">
         <v>1347</v>
       </c>
@@ -74264,7 +74264,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="486" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>422</v>
       </c>
@@ -74335,7 +74335,7 @@
         <v>1742</v>
       </c>
     </row>
-    <row r="487" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>420</v>
       </c>
@@ -74406,7 +74406,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="488" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>322</v>
       </c>
@@ -74480,7 +74480,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="489" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>1100</v>
       </c>
@@ -74551,7 +74551,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="490" spans="1:24" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A490" s="52" t="s">
         <v>1810</v>
       </c>
@@ -74615,7 +74615,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="491" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A491" s="52" t="s">
         <v>1874</v>
       </c>
@@ -74668,7 +74668,7 @@
       <c r="T491" s="54"/>
       <c r="U491" s="54"/>
     </row>
-    <row r="492" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A492" s="52" t="s">
         <v>1879</v>
       </c>
@@ -74739,7 +74739,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="493" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A493" s="52" t="s">
         <v>1882</v>
       </c>
@@ -74810,7 +74810,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="494" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A494" s="52" t="s">
         <v>1887</v>
       </c>
@@ -74881,7 +74881,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="495" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A495" s="52" t="s">
         <v>1890</v>
       </c>
@@ -74952,7 +74952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="496" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A496" s="52" t="s">
         <v>1892</v>
       </c>
@@ -75023,7 +75023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="497" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A497" s="52" t="s">
         <v>1895</v>
       </c>
@@ -75095,7 +75095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="498" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A498" s="52" t="s">
         <v>1897</v>
       </c>
@@ -75148,7 +75148,7 @@
       <c r="T498" s="54"/>
       <c r="U498" s="54"/>
     </row>
-    <row r="499" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A499" s="52" t="s">
         <v>1899</v>
       </c>
@@ -75201,7 +75201,7 @@
       <c r="T499" s="54"/>
       <c r="U499" s="54"/>
     </row>
-    <row r="500" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A500" s="52" t="s">
         <v>1902</v>
       </c>
@@ -75254,7 +75254,7 @@
       <c r="T500" s="54"/>
       <c r="U500" s="54"/>
     </row>
-    <row r="501" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A501" s="52" t="s">
         <v>1904</v>
       </c>
@@ -75309,7 +75309,7 @@
       <c r="T501" s="54"/>
       <c r="U501" s="54"/>
     </row>
-    <row r="502" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A502" s="52" t="s">
         <v>1908</v>
       </c>
@@ -75368,7 +75368,7 @@
       <c r="T502" s="54"/>
       <c r="U502" s="54"/>
     </row>
-    <row r="503" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A503" s="52" t="s">
         <v>1912</v>
       </c>
@@ -75440,7 +75440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="504" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A504" s="52" t="s">
         <v>1920</v>
       </c>
@@ -75493,7 +75493,7 @@
       <c r="T504" s="54"/>
       <c r="U504" s="54"/>
     </row>
-    <row r="505" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A505" s="52" t="s">
         <v>1923</v>
       </c>
@@ -75546,7 +75546,7 @@
       <c r="T505" s="54"/>
       <c r="U505" s="54"/>
     </row>
-    <row r="506" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A506" s="52" t="s">
         <v>1924</v>
       </c>
@@ -75618,7 +75618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="507" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A507" s="52" t="s">
         <v>1927</v>
       </c>
@@ -75686,7 +75686,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="508" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A508" s="52" t="s">
         <v>1929</v>
       </c>
@@ -75758,7 +75758,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="509" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A509" s="52" t="s">
         <v>1931</v>
       </c>
@@ -75830,7 +75830,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="510" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A510" s="52" t="s">
         <v>1933</v>
       </c>
@@ -75902,7 +75902,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="511" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A511" s="52" t="s">
         <v>1935</v>
       </c>
@@ -75974,7 +75974,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="512" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A512" s="52" t="s">
         <v>1938</v>
       </c>
@@ -76046,7 +76046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="513" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A513" s="52" t="s">
         <v>1942</v>
       </c>
@@ -76118,7 +76118,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="514" spans="1:23" ht="43.8" x14ac:dyDescent="0.35">
+    <row r="514" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A514" s="52" t="s">
         <v>1945</v>
       </c>
@@ -76189,7 +76189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="515" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A515" s="52" t="s">
         <v>1949</v>
       </c>
@@ -76260,7 +76260,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="516" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A516" s="52" t="s">
         <v>1953</v>
       </c>
@@ -76331,7 +76331,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="517" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A517" s="52"/>
       <c r="B517" s="54"/>
       <c r="C517" s="54"/>
@@ -76354,111 +76354,111 @@
       <c r="T517" s="54"/>
       <c r="U517" s="54"/>
     </row>
-    <row r="518" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K518" s="8"/>
     </row>
-    <row r="519" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K519" s="8"/>
     </row>
-    <row r="520" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C520" s="8"/>
       <c r="K520" s="8"/>
       <c r="Q520" s="9"/>
     </row>
-    <row r="521" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K521" s="8"/>
     </row>
-    <row r="522" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K522" s="8"/>
       <c r="Q522" s="9"/>
     </row>
-    <row r="523" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K523" s="8"/>
       <c r="Q523" s="9"/>
     </row>
-    <row r="524" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K524" s="8"/>
       <c r="Q524" s="9"/>
     </row>
-    <row r="525" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K525" s="8"/>
       <c r="Q525" s="9"/>
     </row>
-    <row r="526" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K526" s="8"/>
       <c r="Q526" s="9"/>
     </row>
-    <row r="527" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K527" s="8"/>
       <c r="Q527" s="9"/>
     </row>
-    <row r="528" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K528" s="8"/>
       <c r="Q528" s="9"/>
     </row>
-    <row r="529" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="529" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K529" s="8"/>
       <c r="Q529" s="9"/>
     </row>
-    <row r="530" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="530" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K530" s="8"/>
       <c r="Q530" s="9"/>
     </row>
-    <row r="531" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="531" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K531" s="8"/>
       <c r="Q531" s="9"/>
     </row>
-    <row r="532" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="532" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K532" s="8"/>
       <c r="Q532" s="9"/>
     </row>
-    <row r="533" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="533" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K533" s="8"/>
       <c r="Q533" s="9"/>
     </row>
-    <row r="534" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="534" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K534" s="8"/>
       <c r="Q534" s="9"/>
     </row>
-    <row r="535" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="535" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K535" s="8"/>
       <c r="Q535" s="9"/>
     </row>
-    <row r="536" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="536" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K536" s="8"/>
       <c r="Q536" s="9"/>
     </row>
-    <row r="537" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="537" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K537" s="8"/>
     </row>
-    <row r="538" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="538" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K538" s="8"/>
     </row>
-    <row r="539" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="539" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K539" s="8"/>
     </row>
-    <row r="540" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="540" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K540" s="8"/>
     </row>
-    <row r="541" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="541" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K541" s="8"/>
     </row>
-    <row r="542" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="542" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K542" s="8"/>
     </row>
-    <row r="543" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="543" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K543" s="8"/>
     </row>
-    <row r="544" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="544" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K544" s="8"/>
     </row>
-    <row r="545" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="545" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K545" s="8"/>
     </row>
-    <row r="546" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="546" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K546" s="8"/>
     </row>
-    <row r="547" spans="11:17" x14ac:dyDescent="0.3">
+    <row r="547" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K547" s="8"/>
       <c r="Q547" s="9"/>
     </row>

</xml_diff>

<commit_message>
Updating spreadsheets to include additional / updated information.
</commit_message>
<xml_diff>
--- a/megalocytivirus_sequence_data.xlsx
+++ b/megalocytivirus_sequence_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{BD7AB48C-5E6D-4A2E-8E66-70A39FE8C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5D417A-A6B1-4D70-BBED-618D6E03D9E4}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="8_{BD7AB48C-5E6D-4A2E-8E66-70A39FE8C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14F3686-D533-49E1-83E3-AE56651861E0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD6C468C-256F-45C2-B81B-3E7578C677C5}"/>
   </bookViews>
@@ -42208,8 +42208,8 @@
   <dimension ref="A1:Y547"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pane ySplit="1" topLeftCell="A486" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A488" sqref="A488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates alignments and scripts to include whole sequence name in final iqtree trees (rather than only the accession number)
</commit_message>
<xml_diff>
--- a/megalocytivirus_sequence_data.xlsx
+++ b/megalocytivirus_sequence_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="8_{BD7AB48C-5E6D-4A2E-8E66-70A39FE8C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35A47CC1-5E88-476D-AF3D-F063D099DCF8}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="8_{BD7AB48C-5E6D-4A2E-8E66-70A39FE8C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F0D3E33-2B5D-4D22-A825-BD82848C5921}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{CD6C468C-256F-45C2-B81B-3E7578C677C5}"/>
   </bookViews>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9867" uniqueCount="2009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9887" uniqueCount="2020">
   <si>
     <t>Species</t>
   </si>
@@ -41481,12 +41481,45 @@
   <si>
     <t>A comprehensive analysis of the genomic and proteomic profiles of a megalocytivirus isolated from Larimichthys crocea</t>
   </si>
+  <si>
+    <t>MK637631</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>European Chub (Squalius cephalus)</t>
+  </si>
+  <si>
+    <t>Iridoviridae</t>
+  </si>
+  <si>
+    <t>European chub iridovirus</t>
+  </si>
+  <si>
+    <t>ECIV</t>
+  </si>
+  <si>
+    <t>LEC15001</t>
+  </si>
+  <si>
+    <t>Department of Infectious Diseases and             Immunology, University of Florida</t>
+  </si>
+  <si>
+    <t> https://doi.org/10.3390/v11050440</t>
+  </si>
+  <si>
+    <t>Halaly</t>
+  </si>
+  <si>
+    <t>Characterization of a Novel Megalocytivirus Isolated from European Chub (Squalius cephalus)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41668,6 +41701,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -41702,7 +41741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -41837,6 +41876,12 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -42216,9 +42261,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DAEBFD-78AC-4E24-A1EF-CD140122AED7}">
   <dimension ref="A1:Y547"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A486" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B489" sqref="B489"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P288" sqref="P288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42935,7 +42980,7 @@
         <v>47</v>
       </c>
       <c r="I10" t="s">
-        <v>1558</v>
+        <v>1564</v>
       </c>
       <c r="J10" t="s">
         <v>48</v>
@@ -76340,28 +76385,76 @@
         <v>27</v>
       </c>
     </row>
-    <row r="517" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A517" s="52"/>
-      <c r="B517" s="54"/>
-      <c r="C517" s="54"/>
-      <c r="D517" s="55"/>
-      <c r="E517" s="52"/>
-      <c r="F517" s="52"/>
-      <c r="G517" s="58"/>
-      <c r="H517" s="52"/>
-      <c r="I517" s="52"/>
-      <c r="J517" s="52"/>
-      <c r="K517" s="53"/>
-      <c r="L517" s="52"/>
-      <c r="M517" s="54"/>
-      <c r="N517" s="54"/>
-      <c r="O517" s="54"/>
-      <c r="P517" s="52"/>
-      <c r="Q517" s="54"/>
-      <c r="R517" s="57"/>
-      <c r="S517" s="57"/>
-      <c r="T517" s="54"/>
-      <c r="U517" s="54"/>
+    <row r="517" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A517" s="67" t="s">
+        <v>2009</v>
+      </c>
+      <c r="B517" s="54" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C517" s="54" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D517" s="55">
+        <v>2005</v>
+      </c>
+      <c r="E517" s="52" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F517" s="67" t="s">
+        <v>2012</v>
+      </c>
+      <c r="G517" s="52" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H517" s="67" t="s">
+        <v>2013</v>
+      </c>
+      <c r="I517" s="52" t="s">
+        <v>2014</v>
+      </c>
+      <c r="J517" s="67" t="s">
+        <v>2015</v>
+      </c>
+      <c r="K517" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="L517" s="66">
+        <v>128216</v>
+      </c>
+      <c r="M517" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="N517" s="54" t="s">
+        <v>2016</v>
+      </c>
+      <c r="O517" s="33" t="s">
+        <v>2017</v>
+      </c>
+      <c r="P517" s="52" t="s">
+        <v>2018</v>
+      </c>
+      <c r="Q517" s="54" t="s">
+        <v>2019</v>
+      </c>
+      <c r="R517" s="57">
+        <v>2019</v>
+      </c>
+      <c r="S517" s="57" t="s">
+        <v>1960</v>
+      </c>
+      <c r="T517" s="54" t="s">
+        <v>1848</v>
+      </c>
+      <c r="U517" s="54" t="s">
+        <v>1960</v>
+      </c>
+      <c r="V517" s="54" t="s">
+        <v>1960</v>
+      </c>
+      <c r="W517" s="54" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="518" spans="1:23" x14ac:dyDescent="0.3">
       <c r="K518" s="8"/>
@@ -76538,10 +76631,11 @@
     <hyperlink ref="O440" r:id="rId61" xr:uid="{ED368020-7280-453E-A7A5-C8082ECCB50E}"/>
     <hyperlink ref="O486" r:id="rId62" location=":~:text=Whole-genome%20sequences%20of%20RISV-I%20type%20SBIV-VP13%20and%20RSIV-II" xr:uid="{7CFD0E8C-3CB5-4588-A039-B645F7C448E6}"/>
     <hyperlink ref="O489" r:id="rId63" xr:uid="{1F4A9681-B29E-4694-84F5-54C357FA2754}"/>
+    <hyperlink ref="O517" r:id="rId64" display="https://doi.org/10.3390/v11050440" xr:uid="{19A65734-A8F0-409E-9FDC-E966F4495E5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId64"/>
-  <legacyDrawing r:id="rId65"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId65"/>
+  <legacyDrawing r:id="rId66"/>
 </worksheet>
 </file>
 

</xml_diff>